<commit_message>
Refactor: Remove obsolete scripts and update risk history
- Deleted `rebuild-formulas.py`, `test-fmp-earnings.py`, and `test-yfinance-data.py` as they are no longer needed.
- Updated `risk_history.json` to include new risk data for January 20, 2026.
- Added `ARTHUR_CONTEXT.md` to provide project context and strategy details.
- Created `risk_report_20260120.txt` for the latest risk assessment.
- Documented fixes and enhancements in `v1.8-fixes-summary.md`, ensuring alignment with project objectives and improving system reliability.
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions.xlsx
+++ b/projects/fetch-ibkr-positions.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.14353</v>
+        <v>0.14375</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -584,17 +584,17 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M2" t="n">
         <v>1000</v>
       </c>
       <c r="N2" t="n">
-        <v>31.78</v>
+        <v>31.74</v>
       </c>
       <c r="O2" t="n">
-        <v>31780</v>
+        <v>31740</v>
       </c>
       <c r="P2" t="n">
         <v>30.68540181</v>
@@ -606,7 +606,7 @@
         <v>30685.40181</v>
       </c>
       <c r="S2" t="n">
-        <v>1094.59819</v>
+        <v>1054.59819</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="U2" t="n">
-        <v>4561.3834</v>
+        <v>4562.625</v>
       </c>
     </row>
     <row r="3">
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.1599</v>
+        <v>1.1645</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -643,12 +643,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MC</t>
+          <t>RMS</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>LVMH MOET HENNESSY LOUIS VUI</t>
+          <t>HERMES INTL</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -659,29 +659,29 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="N3" t="n">
-        <v>609.2</v>
+        <v>2113</v>
       </c>
       <c r="O3" t="n">
-        <v>6092</v>
+        <v>6339</v>
       </c>
       <c r="P3" t="n">
-        <v>625.9127999999999</v>
+        <v>2126.0625</v>
       </c>
       <c r="Q3" t="n">
-        <v>625.9127999999999</v>
+        <v>2126.0625</v>
       </c>
       <c r="R3" t="n">
-        <v>6259.128</v>
+        <v>6378.1875</v>
       </c>
       <c r="S3" t="n">
-        <v>-167.128</v>
+        <v>-39.1875</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="U3" t="n">
-        <v>7066.110799999999</v>
+        <v>7381.7655</v>
       </c>
     </row>
     <row r="4">
@@ -700,11 +700,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>SGD</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.1599</v>
+        <v>0.77833</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -713,17 +713,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>RMS</t>
+          <t>ES3</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>HERMES INTL</t>
+          <t>SPDR STRAITS TIMES INDEX ETF</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -734,29 +734,29 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>5000</v>
       </c>
       <c r="N4" t="n">
-        <v>2190</v>
+        <v>4.905</v>
       </c>
       <c r="O4" t="n">
-        <v>6570</v>
+        <v>24525</v>
       </c>
       <c r="P4" t="n">
-        <v>2126.0625</v>
+        <v>4.54124249</v>
       </c>
       <c r="Q4" t="n">
-        <v>2126.0625</v>
+        <v>4.54124249</v>
       </c>
       <c r="R4" t="n">
-        <v>6378.1875</v>
+        <v>22706.21245</v>
       </c>
       <c r="S4" t="n">
-        <v>191.8125</v>
+        <v>1818.78755</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
@@ -764,7 +764,7 @@
         </is>
       </c>
       <c r="U4" t="n">
-        <v>7620.543</v>
+        <v>19088.54325</v>
       </c>
     </row>
     <row r="5">
@@ -779,7 +779,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.77579</v>
+        <v>0.77833</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -793,12 +793,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ES3</t>
+          <t>GSD</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>SPDR STRAITS TIMES INDEX ETF</t>
+          <t>SPDR GOLD SHARES</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -809,29 +809,29 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>5000</v>
+        <v>50</v>
       </c>
       <c r="N5" t="n">
-        <v>4.927</v>
+        <v>552.1</v>
       </c>
       <c r="O5" t="n">
-        <v>24635</v>
+        <v>27605</v>
       </c>
       <c r="P5" t="n">
-        <v>4.54124249</v>
+        <v>432.4596912</v>
       </c>
       <c r="Q5" t="n">
-        <v>4.54124249</v>
+        <v>432.4596912</v>
       </c>
       <c r="R5" t="n">
-        <v>22706.21245</v>
+        <v>21622.98456</v>
       </c>
       <c r="S5" t="n">
-        <v>1928.78755</v>
+        <v>5982.01544</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -839,7 +839,7 @@
         </is>
       </c>
       <c r="U5" t="n">
-        <v>19111.58665</v>
+        <v>21485.79965</v>
       </c>
     </row>
     <row r="6">
@@ -850,11 +850,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.77579</v>
+        <v>1</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -863,17 +863,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>GSD</t>
+          <t>AMZN</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>SPDR GOLD SHARES</t>
+          <t>AMAZON.COM INC</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -884,29 +884,29 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N6" t="n">
-        <v>545.45</v>
+        <v>239.12</v>
       </c>
       <c r="O6" t="n">
-        <v>27272.5</v>
+        <v>23912</v>
       </c>
       <c r="P6" t="n">
-        <v>432.4596912</v>
+        <v>216.590322</v>
       </c>
       <c r="Q6" t="n">
-        <v>432.4596912</v>
+        <v>216.590322</v>
       </c>
       <c r="R6" t="n">
-        <v>21622.98456</v>
+        <v>21659.0322</v>
       </c>
       <c r="S6" t="n">
-        <v>5649.51544</v>
+        <v>2252.9678</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="U6" t="n">
-        <v>21157.732775</v>
+        <v>23912</v>
       </c>
     </row>
     <row r="7">
@@ -938,17 +938,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>AMZN</t>
+          <t>BITO</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>AMAZON.COM INC</t>
+          <t>PROSHARES BITCOIN ETF-USD</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -959,29 +959,29 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M7" t="n">
         <v>100</v>
       </c>
       <c r="N7" t="n">
-        <v>239.12</v>
+        <v>13.26</v>
       </c>
       <c r="O7" t="n">
-        <v>23912</v>
+        <v>1326</v>
       </c>
       <c r="P7" t="n">
-        <v>216.590322</v>
+        <v>12.97</v>
       </c>
       <c r="Q7" t="n">
-        <v>216.590322</v>
+        <v>12.97</v>
       </c>
       <c r="R7" t="n">
-        <v>21659.0322</v>
+        <v>1297</v>
       </c>
       <c r="S7" t="n">
-        <v>2252.9678</v>
+        <v>29</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -989,7 +989,7 @@
         </is>
       </c>
       <c r="U7" t="n">
-        <v>23912</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="8">
@@ -1013,17 +1013,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>BITO</t>
+          <t>CELH</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>PROSHARES BITCOIN ETF-USD</t>
+          <t>CELSIUS HOLDINGS INC</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -1034,29 +1034,29 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N8" t="n">
-        <v>13.26</v>
+        <v>54.39</v>
       </c>
       <c r="O8" t="n">
-        <v>1326</v>
+        <v>2719.5</v>
       </c>
       <c r="P8" t="n">
-        <v>12.97</v>
+        <v>46.285022</v>
       </c>
       <c r="Q8" t="n">
-        <v>12.97</v>
+        <v>46.285022</v>
       </c>
       <c r="R8" t="n">
-        <v>1297</v>
+        <v>2314.2511</v>
       </c>
       <c r="S8" t="n">
-        <v>29</v>
+        <v>405.2489</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
@@ -1064,7 +1064,7 @@
         </is>
       </c>
       <c r="U8" t="n">
-        <v>1326</v>
+        <v>2719.5</v>
       </c>
     </row>
     <row r="9">
@@ -1088,17 +1088,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ADR</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>CELH</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>CELSIUS HOLDINGS INC</t>
+          <t>CHAGEE HOLDINGS LTD-ADR</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -1109,29 +1109,29 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N9" t="n">
-        <v>54.39</v>
+        <v>12.09</v>
       </c>
       <c r="O9" t="n">
-        <v>2719.5</v>
+        <v>1209</v>
       </c>
       <c r="P9" t="n">
-        <v>46.285022</v>
+        <v>12.49</v>
       </c>
       <c r="Q9" t="n">
-        <v>46.285022</v>
+        <v>12.49</v>
       </c>
       <c r="R9" t="n">
-        <v>2314.2511</v>
+        <v>1249</v>
       </c>
       <c r="S9" t="n">
-        <v>405.2489</v>
+        <v>-40</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1139,7 +1139,7 @@
         </is>
       </c>
       <c r="U9" t="n">
-        <v>2719.5</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="10">
@@ -1163,17 +1163,17 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>ADR</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>CSNDX</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>CHAGEE HOLDINGS LTD-ADR</t>
+          <t>ISHARES NASDAQ 100 USD ACC</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -1184,29 +1184,29 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N10" t="n">
-        <v>12.09</v>
+        <v>1444</v>
       </c>
       <c r="O10" t="n">
-        <v>1209</v>
+        <v>14440</v>
       </c>
       <c r="P10" t="n">
-        <v>12.49</v>
+        <v>1476.8770695</v>
       </c>
       <c r="Q10" t="n">
-        <v>12.49</v>
+        <v>1476.8770695</v>
       </c>
       <c r="R10" t="n">
-        <v>1249</v>
+        <v>14768.770695</v>
       </c>
       <c r="S10" t="n">
-        <v>-40</v>
+        <v>-328.770695</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -1214,7 +1214,7 @@
         </is>
       </c>
       <c r="U10" t="n">
-        <v>1209</v>
+        <v>14440</v>
       </c>
     </row>
     <row r="11">
@@ -1243,12 +1243,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>CSNDX</t>
+          <t>CTEC</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ISHARES NASDAQ 100 USD ACC</t>
+          <t>ISHARES CHINA TECH USD ACC</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -1259,29 +1259,29 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>10</v>
+        <v>2000</v>
       </c>
       <c r="N11" t="n">
-        <v>1468</v>
+        <v>5.488</v>
       </c>
       <c r="O11" t="n">
-        <v>14680</v>
+        <v>10976</v>
       </c>
       <c r="P11" t="n">
-        <v>1476.8770695</v>
+        <v>5.5697835</v>
       </c>
       <c r="Q11" t="n">
-        <v>1476.8770695</v>
+        <v>5.5697835</v>
       </c>
       <c r="R11" t="n">
-        <v>14768.770695</v>
+        <v>11139.567</v>
       </c>
       <c r="S11" t="n">
-        <v>-88.770695</v>
+        <v>-163.567</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="U11" t="n">
-        <v>14680</v>
+        <v>10976</v>
       </c>
     </row>
     <row r="12">
@@ -1313,17 +1313,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>CTEC</t>
+          <t>GOOGL</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>ISHARES CHINA TECH USD ACC</t>
+          <t>ALPHABET INC-CL A</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1334,29 +1334,29 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="N12" t="n">
-        <v>5.473</v>
+        <v>330</v>
       </c>
       <c r="O12" t="n">
-        <v>10946</v>
+        <v>33000</v>
       </c>
       <c r="P12" t="n">
-        <v>5.5697835</v>
+        <v>312.15</v>
       </c>
       <c r="Q12" t="n">
-        <v>5.5697835</v>
+        <v>312.15</v>
       </c>
       <c r="R12" t="n">
-        <v>11139.567</v>
+        <v>31215</v>
       </c>
       <c r="S12" t="n">
-        <v>-193.567</v>
+        <v>1785</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
@@ -1364,7 +1364,7 @@
         </is>
       </c>
       <c r="U12" t="n">
-        <v>10946</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="13">
@@ -1393,12 +1393,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>GOOGL</t>
+          <t>GRAB</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>ALPHABET INC-CL A</t>
+          <t>GRAB HOLDINGS LTD - CL A</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1409,29 +1409,29 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="N13" t="n">
-        <v>330</v>
+        <v>4.38</v>
       </c>
       <c r="O13" t="n">
-        <v>33000</v>
+        <v>2190</v>
       </c>
       <c r="P13" t="n">
-        <v>312.15</v>
+        <v>5.166</v>
       </c>
       <c r="Q13" t="n">
-        <v>312.15</v>
+        <v>5.166</v>
       </c>
       <c r="R13" t="n">
-        <v>31215</v>
+        <v>2583</v>
       </c>
       <c r="S13" t="n">
-        <v>1785</v>
+        <v>-393</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -1439,7 +1439,7 @@
         </is>
       </c>
       <c r="U13" t="n">
-        <v>33000</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="14">
@@ -1463,17 +1463,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>GRAB</t>
+          <t>HEAL</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>GRAB HOLDINGS LTD - CL A</t>
+          <t>ISHR HEALTHCARE INNOVATION</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1484,29 +1484,29 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N14" t="n">
-        <v>4.38</v>
+        <v>9.2675</v>
       </c>
       <c r="O14" t="n">
-        <v>2190</v>
+        <v>9267.5</v>
       </c>
       <c r="P14" t="n">
-        <v>5.166</v>
+        <v>9.424709999999999</v>
       </c>
       <c r="Q14" t="n">
-        <v>5.166</v>
+        <v>9.424709999999999</v>
       </c>
       <c r="R14" t="n">
-        <v>2583</v>
+        <v>9424.709999999999</v>
       </c>
       <c r="S14" t="n">
-        <v>-393</v>
+        <v>-157.21</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
@@ -1514,7 +1514,7 @@
         </is>
       </c>
       <c r="U14" t="n">
-        <v>2190</v>
+        <v>9267.5</v>
       </c>
     </row>
     <row r="15">
@@ -1543,12 +1543,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>HEAL</t>
+          <t>INRA</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ISHR HEALTHCARE INNOVATION</t>
+          <t>ISHAR GL CL EN TR UCI ETF-US</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1559,29 +1559,29 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>1000</v>
+        <v>385</v>
       </c>
       <c r="N15" t="n">
-        <v>9.42</v>
+        <v>25.9392</v>
       </c>
       <c r="O15" t="n">
-        <v>9420</v>
+        <v>9986.59</v>
       </c>
       <c r="P15" t="n">
-        <v>9.424709999999999</v>
+        <v>26.012734603</v>
       </c>
       <c r="Q15" t="n">
-        <v>9.424709999999999</v>
+        <v>26.012734603</v>
       </c>
       <c r="R15" t="n">
-        <v>9424.709999999999</v>
+        <v>10014.902822</v>
       </c>
       <c r="S15" t="n">
-        <v>-4.71</v>
+        <v>-28.312822</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -1589,7 +1589,7 @@
         </is>
       </c>
       <c r="U15" t="n">
-        <v>9420</v>
+        <v>9986.59</v>
       </c>
     </row>
     <row r="16">
@@ -1613,17 +1613,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>ADR</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>INRA</t>
+          <t>LKNCY</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>ISHAR GL CL EN TR UCI ETF-US</t>
+          <t>LUCKIN COFFEE INC - ADR</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1634,29 +1634,29 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>385</v>
+        <v>50</v>
       </c>
       <c r="N16" t="n">
-        <v>26.1068</v>
+        <v>33.95</v>
       </c>
       <c r="O16" t="n">
-        <v>10051.12</v>
+        <v>1697.5</v>
       </c>
       <c r="P16" t="n">
-        <v>26.012734603</v>
+        <v>36.96000022</v>
       </c>
       <c r="Q16" t="n">
-        <v>26.012734603</v>
+        <v>36.96000022</v>
       </c>
       <c r="R16" t="n">
-        <v>10014.902822</v>
+        <v>1848.000011</v>
       </c>
       <c r="S16" t="n">
-        <v>36.217178</v>
+        <v>-150.500011</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
@@ -1664,7 +1664,7 @@
         </is>
       </c>
       <c r="U16" t="n">
-        <v>10051.12</v>
+        <v>1697.5</v>
       </c>
     </row>
     <row r="17">
@@ -1688,17 +1688,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ADR</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>LKNCY</t>
+          <t>LOCK</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>LUCKIN COFFEE INC - ADR</t>
+          <t>ISHARES DIGITAL SCRTY USD-A</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1709,29 +1709,29 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="N17" t="n">
-        <v>33.95</v>
+        <v>9.939</v>
       </c>
       <c r="O17" t="n">
-        <v>1697.5</v>
+        <v>9939</v>
       </c>
       <c r="P17" t="n">
-        <v>36.96000022</v>
+        <v>10.2267108</v>
       </c>
       <c r="Q17" t="n">
-        <v>36.96000022</v>
+        <v>10.2267108</v>
       </c>
       <c r="R17" t="n">
-        <v>1848.000011</v>
+        <v>10226.7108</v>
       </c>
       <c r="S17" t="n">
-        <v>-150.500011</v>
+        <v>-287.7108</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
@@ -1739,7 +1739,7 @@
         </is>
       </c>
       <c r="U17" t="n">
-        <v>1697.5</v>
+        <v>9939</v>
       </c>
     </row>
     <row r="18">
@@ -1763,17 +1763,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>LOCK</t>
+          <t>LULU</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>ISHARES DIGITAL SCRTY USD-A</t>
+          <t>LULULEMON ATHLETICA INC</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1784,29 +1784,29 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>1000</v>
+        <v>40</v>
       </c>
       <c r="N18" t="n">
-        <v>10.127</v>
+        <v>201.87</v>
       </c>
       <c r="O18" t="n">
-        <v>10127</v>
+        <v>8074.8</v>
       </c>
       <c r="P18" t="n">
-        <v>10.2267108</v>
+        <v>186.05813325</v>
       </c>
       <c r="Q18" t="n">
-        <v>10.2267108</v>
+        <v>186.05813325</v>
       </c>
       <c r="R18" t="n">
-        <v>10226.7108</v>
+        <v>7442.32533</v>
       </c>
       <c r="S18" t="n">
-        <v>-99.71080000000001</v>
+        <v>632.4746699999999</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
@@ -1814,7 +1814,7 @@
         </is>
       </c>
       <c r="U18" t="n">
-        <v>10127</v>
+        <v>8074.8</v>
       </c>
     </row>
     <row r="19">
@@ -1843,12 +1843,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>LULU</t>
+          <t>MELI</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>LULULEMON ATHLETICA INC</t>
+          <t>MERCADOLIBRE INC</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1859,29 +1859,29 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="N19" t="n">
-        <v>201.87</v>
+        <v>2075.01</v>
       </c>
       <c r="O19" t="n">
-        <v>8074.8</v>
+        <v>2075.01</v>
       </c>
       <c r="P19" t="n">
-        <v>186.05813325</v>
+        <v>2086.200022</v>
       </c>
       <c r="Q19" t="n">
-        <v>186.05813325</v>
+        <v>2086.200022</v>
       </c>
       <c r="R19" t="n">
-        <v>7442.32533</v>
+        <v>2086.200022</v>
       </c>
       <c r="S19" t="n">
-        <v>632.4746699999999</v>
+        <v>-11.190022</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
@@ -1889,7 +1889,7 @@
         </is>
       </c>
       <c r="U19" t="n">
-        <v>8074.8</v>
+        <v>2075.01</v>
       </c>
     </row>
     <row r="20">
@@ -1918,12 +1918,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>MELI</t>
+          <t>NVDA</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>MERCADOLIBRE INC</t>
+          <t>NVIDIA CORP</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1934,29 +1934,29 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="N20" t="n">
-        <v>2075.01</v>
+        <v>186.23</v>
       </c>
       <c r="O20" t="n">
-        <v>2075.01</v>
+        <v>37246</v>
       </c>
       <c r="P20" t="n">
-        <v>2086.200022</v>
+        <v>185.216422</v>
       </c>
       <c r="Q20" t="n">
-        <v>2086.200022</v>
+        <v>185.216422</v>
       </c>
       <c r="R20" t="n">
-        <v>2086.200022</v>
+        <v>37043.2844</v>
       </c>
       <c r="S20" t="n">
-        <v>-11.190022</v>
+        <v>202.7156</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
@@ -1964,7 +1964,7 @@
         </is>
       </c>
       <c r="U20" t="n">
-        <v>2075.01</v>
+        <v>37246</v>
       </c>
     </row>
     <row r="21">
@@ -1993,12 +1993,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>ORCL</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>NVIDIA CORP</t>
+          <t>ORACLE CORP</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -2009,29 +2009,29 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N21" t="n">
-        <v>186.23</v>
+        <v>191.09</v>
       </c>
       <c r="O21" t="n">
-        <v>37246</v>
+        <v>19109</v>
       </c>
       <c r="P21" t="n">
-        <v>185.216422</v>
+        <v>205.3357044</v>
       </c>
       <c r="Q21" t="n">
-        <v>185.216422</v>
+        <v>205.3357044</v>
       </c>
       <c r="R21" t="n">
-        <v>37043.2844</v>
+        <v>20533.57044</v>
       </c>
       <c r="S21" t="n">
-        <v>202.7156</v>
+        <v>-1424.57044</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
@@ -2039,7 +2039,7 @@
         </is>
       </c>
       <c r="U21" t="n">
-        <v>37246</v>
+        <v>19109</v>
       </c>
     </row>
     <row r="22">
@@ -2063,17 +2063,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ADR</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ORCL</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>ORACLE CORP</t>
+          <t>SEA LTD-ADR</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -2084,29 +2084,29 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N22" t="n">
-        <v>191.09</v>
+        <v>121.42</v>
       </c>
       <c r="O22" t="n">
-        <v>19109</v>
+        <v>1214.2</v>
       </c>
       <c r="P22" t="n">
-        <v>205.3357044</v>
+        <v>128.6</v>
       </c>
       <c r="Q22" t="n">
-        <v>205.3357044</v>
+        <v>128.6</v>
       </c>
       <c r="R22" t="n">
-        <v>20533.57044</v>
+        <v>1286</v>
       </c>
       <c r="S22" t="n">
-        <v>-1424.57044</v>
+        <v>-71.8</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
@@ -2114,7 +2114,7 @@
         </is>
       </c>
       <c r="U22" t="n">
-        <v>19109</v>
+        <v>1214.2</v>
       </c>
     </row>
     <row r="23">
@@ -2138,17 +2138,17 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ADR</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>VWRA</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>SEA LTD-ADR</t>
+          <t>VANG FTSE AW USDA</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -2159,29 +2159,29 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>10</v>
+        <v>600</v>
       </c>
       <c r="N23" t="n">
-        <v>121.42</v>
+        <v>172.46</v>
       </c>
       <c r="O23" t="n">
-        <v>1214.2</v>
+        <v>103476</v>
       </c>
       <c r="P23" t="n">
-        <v>128.6</v>
+        <v>170.213547575</v>
       </c>
       <c r="Q23" t="n">
-        <v>128.6</v>
+        <v>170.213547575</v>
       </c>
       <c r="R23" t="n">
-        <v>1286</v>
+        <v>102128.128545</v>
       </c>
       <c r="S23" t="n">
-        <v>-71.8</v>
+        <v>1347.871455</v>
       </c>
       <c r="T23" t="inlineStr">
         <is>
@@ -2189,7 +2189,7 @@
         </is>
       </c>
       <c r="U23" t="n">
-        <v>1214.2</v>
+        <v>103476</v>
       </c>
     </row>
     <row r="24">
@@ -2208,55 +2208,65 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>FOP</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>VWRA</t>
+          <t>EW2G6 P6525</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>VANG FTSE AW USDA</t>
+          <t>ES 13FEB26 6525 P</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
-      </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+        <v>50</v>
+      </c>
+      <c r="I24" t="n">
+        <v>6525</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>600</v>
+        <v>2</v>
       </c>
       <c r="N24" t="n">
-        <v>173.84</v>
+        <v>19</v>
       </c>
       <c r="O24" t="n">
-        <v>104304</v>
+        <v>1900</v>
       </c>
       <c r="P24" t="n">
-        <v>170.213547575</v>
+        <v>31.5284</v>
       </c>
       <c r="Q24" t="n">
-        <v>170.213547575</v>
+        <v>31.5284</v>
       </c>
       <c r="R24" t="n">
-        <v>102128.128545</v>
+        <v>3152.84</v>
       </c>
       <c r="S24" t="n">
-        <v>2175.871455</v>
+        <v>-1252.84</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
@@ -2264,7 +2274,7 @@
         </is>
       </c>
       <c r="U24" t="n">
-        <v>104304</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="25">
@@ -2288,24 +2298,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>EW2G6 P6525</t>
+          <t>EW2G6 C7300</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>ES 13FEB26 6525 P</t>
+          <t>ES 13FEB26 7300 C</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>50</v>
       </c>
       <c r="I25" t="n">
-        <v>6525</v>
+        <v>7300</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2314,34 +2324,34 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M25" t="n">
         <v>2</v>
       </c>
       <c r="N25" t="n">
-        <v>19</v>
+        <v>3.5</v>
       </c>
       <c r="O25" t="n">
-        <v>1900</v>
+        <v>350</v>
       </c>
       <c r="P25" t="n">
-        <v>31.5284</v>
+        <v>8.0284</v>
       </c>
       <c r="Q25" t="n">
-        <v>31.5284</v>
+        <v>8.0284</v>
       </c>
       <c r="R25" t="n">
-        <v>3152.84</v>
+        <v>802.84</v>
       </c>
       <c r="S25" t="n">
-        <v>-1252.84</v>
+        <v>-452.84</v>
       </c>
       <c r="T25" t="inlineStr">
         <is>
@@ -2349,7 +2359,7 @@
         </is>
       </c>
       <c r="U25" t="n">
-        <v>1900</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26">
@@ -2368,73 +2378,73 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>FOP</t>
+          <t>OPT</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>EW2G6 C7300</t>
+          <t>AAPL  260130P00250000</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>ES 13FEB26 7300 C</t>
+          <t>AAPL 30JAN26 250 P</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I26" t="n">
-        <v>7300</v>
+        <v>250</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="N26" t="n">
-        <v>3.5</v>
+        <v>3.55</v>
       </c>
       <c r="O26" t="n">
-        <v>350</v>
+        <v>-355</v>
       </c>
       <c r="P26" t="n">
-        <v>8.0284</v>
+        <v>3.0594796</v>
       </c>
       <c r="Q26" t="n">
-        <v>8.0284</v>
+        <v>3.0594796</v>
       </c>
       <c r="R26" t="n">
-        <v>802.84</v>
+        <v>-305.94796</v>
       </c>
       <c r="S26" t="n">
-        <v>-452.84</v>
+        <v>-49.05204</v>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>Long</t>
+          <t>Short</t>
         </is>
       </c>
       <c r="U26" t="n">
-        <v>350</v>
+        <v>-355</v>
       </c>
     </row>
     <row r="27">
@@ -2463,23 +2473,23 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>AAPL  260130P00250000</t>
+          <t>AMZN  260220P00215000</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>AAPL 30JAN26 250 P</t>
+          <t>AMZN 20FEB26 215 P</t>
         </is>
       </c>
       <c r="H27" t="n">
         <v>100</v>
       </c>
       <c r="I27" t="n">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2489,29 +2499,29 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M27" t="n">
         <v>-1</v>
       </c>
       <c r="N27" t="n">
-        <v>3.55</v>
+        <v>2.715</v>
       </c>
       <c r="O27" t="n">
-        <v>-355</v>
+        <v>-271.5</v>
       </c>
       <c r="P27" t="n">
-        <v>3.0594796</v>
+        <v>4.3794796</v>
       </c>
       <c r="Q27" t="n">
-        <v>3.0594796</v>
+        <v>4.3794796</v>
       </c>
       <c r="R27" t="n">
-        <v>-305.94796</v>
+        <v>-437.94796</v>
       </c>
       <c r="S27" t="n">
-        <v>-49.05204</v>
+        <v>166.44796</v>
       </c>
       <c r="T27" t="inlineStr">
         <is>
@@ -2519,7 +2529,7 @@
         </is>
       </c>
       <c r="U27" t="n">
-        <v>-355</v>
+        <v>-271.5</v>
       </c>
     </row>
     <row r="28">
@@ -2543,60 +2553,60 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>AMZN  260220P00215000</t>
+          <t>AMZN  260227C00255000</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>AMZN 20FEB26 215 P</t>
+          <t>AMZN 27FEB26 255 C</t>
         </is>
       </c>
       <c r="H28" t="n">
         <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>215</v>
+        <v>255</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-27</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M28" t="n">
         <v>-1</v>
       </c>
       <c r="N28" t="n">
-        <v>2.715</v>
+        <v>5.5</v>
       </c>
       <c r="O28" t="n">
-        <v>-271.5</v>
+        <v>-550</v>
       </c>
       <c r="P28" t="n">
-        <v>4.3794796</v>
+        <v>5.4294796</v>
       </c>
       <c r="Q28" t="n">
-        <v>4.3794796</v>
+        <v>5.4294796</v>
       </c>
       <c r="R28" t="n">
-        <v>-437.94796</v>
+        <v>-542.94796</v>
       </c>
       <c r="S28" t="n">
-        <v>166.44796</v>
+        <v>-7.05204</v>
       </c>
       <c r="T28" t="inlineStr">
         <is>
@@ -2604,7 +2614,7 @@
         </is>
       </c>
       <c r="U28" t="n">
-        <v>-271.5</v>
+        <v>-550</v>
       </c>
     </row>
     <row r="29">
@@ -2628,24 +2638,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>AMZN  260227C00255000</t>
+          <t>GOOGL 260227P00310000</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>AMZN 27FEB26 255 C</t>
+          <t>GOOGL 27FEB26 310 P</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>100</v>
       </c>
       <c r="I29" t="n">
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2654,34 +2664,34 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M29" t="n">
         <v>-1</v>
       </c>
       <c r="N29" t="n">
-        <v>5.5</v>
+        <v>6.975</v>
       </c>
       <c r="O29" t="n">
-        <v>-550</v>
+        <v>-697.5</v>
       </c>
       <c r="P29" t="n">
-        <v>5.4294796</v>
+        <v>7.2294546</v>
       </c>
       <c r="Q29" t="n">
-        <v>5.4294796</v>
+        <v>7.2294546</v>
       </c>
       <c r="R29" t="n">
-        <v>-542.94796</v>
+        <v>-722.94546</v>
       </c>
       <c r="S29" t="n">
-        <v>-7.05204</v>
+        <v>25.44546</v>
       </c>
       <c r="T29" t="inlineStr">
         <is>
@@ -2689,7 +2699,7 @@
         </is>
       </c>
       <c r="U29" t="n">
-        <v>-550</v>
+        <v>-697.5</v>
       </c>
     </row>
     <row r="30">
@@ -2713,24 +2723,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>GOOGL 260227P00310000</t>
+          <t>GOOGL 260227C00370000</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>GOOGL 27FEB26 310 P</t>
+          <t>GOOGL 27FEB26 370 C</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>100</v>
       </c>
       <c r="I30" t="n">
-        <v>310</v>
+        <v>370</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2739,34 +2749,34 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M30" t="n">
         <v>-1</v>
       </c>
       <c r="N30" t="n">
-        <v>6.975</v>
+        <v>3.65</v>
       </c>
       <c r="O30" t="n">
-        <v>-697.5</v>
+        <v>-365</v>
       </c>
       <c r="P30" t="n">
-        <v>7.2294546</v>
+        <v>5.6494546</v>
       </c>
       <c r="Q30" t="n">
-        <v>7.2294546</v>
+        <v>5.6494546</v>
       </c>
       <c r="R30" t="n">
-        <v>-722.94546</v>
+        <v>-564.94546</v>
       </c>
       <c r="S30" t="n">
-        <v>25.44546</v>
+        <v>199.94546</v>
       </c>
       <c r="T30" t="inlineStr">
         <is>
@@ -2774,7 +2784,7 @@
         </is>
       </c>
       <c r="U30" t="n">
-        <v>-697.5</v>
+        <v>-365</v>
       </c>
     </row>
     <row r="31">
@@ -2798,60 +2808,60 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>GOOGL 260227C00370000</t>
+          <t>JPM   260206P00300000</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>GOOGL 27FEB26 370 C</t>
+          <t>JPM 06FEB26 300 P</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>370</v>
+        <v>300</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2026-02-27</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M31" t="n">
         <v>-1</v>
       </c>
       <c r="N31" t="n">
-        <v>3.65</v>
+        <v>2.185</v>
       </c>
       <c r="O31" t="n">
-        <v>-365</v>
+        <v>-218.5</v>
       </c>
       <c r="P31" t="n">
-        <v>5.6494546</v>
+        <v>2.4194546</v>
       </c>
       <c r="Q31" t="n">
-        <v>5.6494546</v>
+        <v>2.4194546</v>
       </c>
       <c r="R31" t="n">
-        <v>-564.94546</v>
+        <v>-241.94546</v>
       </c>
       <c r="S31" t="n">
-        <v>199.94546</v>
+        <v>23.44546</v>
       </c>
       <c r="T31" t="inlineStr">
         <is>
@@ -2859,7 +2869,7 @@
         </is>
       </c>
       <c r="U31" t="n">
-        <v>-365</v>
+        <v>-218.5</v>
       </c>
     </row>
     <row r="32">
@@ -2883,60 +2893,60 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>JPM   260206P00300000</t>
+          <t>NVDA  260130C00195000</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>JPM 06FEB26 300 P</t>
+          <t>NVDA 30JAN26 195 C</t>
         </is>
       </c>
       <c r="H32" t="n">
         <v>100</v>
       </c>
       <c r="I32" t="n">
-        <v>300</v>
+        <v>195</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N32" t="n">
-        <v>2.185</v>
+        <v>1.78</v>
       </c>
       <c r="O32" t="n">
-        <v>-218.5</v>
+        <v>-356</v>
       </c>
       <c r="P32" t="n">
-        <v>2.4194546</v>
+        <v>2.1886796</v>
       </c>
       <c r="Q32" t="n">
-        <v>2.4194546</v>
+        <v>2.1886796</v>
       </c>
       <c r="R32" t="n">
-        <v>-241.94546</v>
+        <v>-437.73592</v>
       </c>
       <c r="S32" t="n">
-        <v>23.44546</v>
+        <v>81.73591999999999</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
@@ -2944,7 +2954,7 @@
         </is>
       </c>
       <c r="U32" t="n">
-        <v>-218.5</v>
+        <v>-356</v>
       </c>
     </row>
     <row r="33">
@@ -2973,12 +2983,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>NVDA  260130C00195000</t>
+          <t>ORCL  260123C00195000</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>NVDA 30JAN26 195 C</t>
+          <t>ORCL 23JAN26 195 C</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -2989,7 +2999,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2999,29 +3009,29 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="N33" t="n">
-        <v>1.78</v>
+        <v>2.755</v>
       </c>
       <c r="O33" t="n">
-        <v>-356</v>
+        <v>-275.5</v>
       </c>
       <c r="P33" t="n">
-        <v>2.1886796</v>
+        <v>1.7325796</v>
       </c>
       <c r="Q33" t="n">
-        <v>2.1886796</v>
+        <v>1.7325796</v>
       </c>
       <c r="R33" t="n">
-        <v>-437.73592</v>
+        <v>-173.25796</v>
       </c>
       <c r="S33" t="n">
-        <v>81.73591999999999</v>
+        <v>-102.24204</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
@@ -3029,7 +3039,7 @@
         </is>
       </c>
       <c r="U33" t="n">
-        <v>-356</v>
+        <v>-275.5</v>
       </c>
     </row>
     <row r="34">
@@ -3048,65 +3058,65 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>OPT</t>
+          <t>FOP</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>ORCL  260123C00195000</t>
+          <t>EW2G6 P6625</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>ORCL 23JAN26 195 C</t>
+          <t>ES 13FEB26 6625 P</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I34" t="n">
-        <v>195</v>
+        <v>6625</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N34" t="n">
-        <v>2.755</v>
+        <v>26.25</v>
       </c>
       <c r="O34" t="n">
-        <v>-275.5</v>
+        <v>-2625</v>
       </c>
       <c r="P34" t="n">
-        <v>1.7325796</v>
+        <v>42.2216</v>
       </c>
       <c r="Q34" t="n">
-        <v>1.7325796</v>
+        <v>42.2216</v>
       </c>
       <c r="R34" t="n">
-        <v>-173.25796</v>
+        <v>-4222.16</v>
       </c>
       <c r="S34" t="n">
-        <v>-102.24204</v>
+        <v>1597.16</v>
       </c>
       <c r="T34" t="inlineStr">
         <is>
@@ -3114,7 +3124,7 @@
         </is>
       </c>
       <c r="U34" t="n">
-        <v>-275.5</v>
+        <v>-2625</v>
       </c>
     </row>
     <row r="35">
@@ -3138,24 +3148,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>EW2G6 P6625</t>
+          <t>EW2G6 C7200</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>ES 13FEB26 6625 P</t>
+          <t>ES 13FEB26 7200 C</t>
         </is>
       </c>
       <c r="H35" t="n">
         <v>50</v>
       </c>
       <c r="I35" t="n">
-        <v>6625</v>
+        <v>7200</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3164,34 +3174,34 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M35" t="n">
         <v>-2</v>
       </c>
       <c r="N35" t="n">
-        <v>26.25</v>
+        <v>12.25</v>
       </c>
       <c r="O35" t="n">
-        <v>-2625</v>
+        <v>-1225</v>
       </c>
       <c r="P35" t="n">
-        <v>42.2216</v>
+        <v>18.9716</v>
       </c>
       <c r="Q35" t="n">
-        <v>42.2216</v>
+        <v>18.9716</v>
       </c>
       <c r="R35" t="n">
-        <v>-4222.16</v>
+        <v>-1897.16</v>
       </c>
       <c r="S35" t="n">
-        <v>1597.16</v>
+        <v>672.16</v>
       </c>
       <c r="T35" t="inlineStr">
         <is>
@@ -3199,91 +3209,6 @@
         </is>
       </c>
       <c r="U35" t="n">
-        <v>-2625</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>U2739721</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>1</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>FOP</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>EW2G6 C7200</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>ES 13FEB26 7200 C</t>
-        </is>
-      </c>
-      <c r="H36" t="n">
-        <v>50</v>
-      </c>
-      <c r="I36" t="n">
-        <v>7200</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>2026-02-13</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>2026-01-16</t>
-        </is>
-      </c>
-      <c r="M36" t="n">
-        <v>-2</v>
-      </c>
-      <c r="N36" t="n">
-        <v>12.25</v>
-      </c>
-      <c r="O36" t="n">
-        <v>-1225</v>
-      </c>
-      <c r="P36" t="n">
-        <v>18.9716</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>18.9716</v>
-      </c>
-      <c r="R36" t="n">
-        <v>-1897.16</v>
-      </c>
-      <c r="S36" t="n">
-        <v>672.16</v>
-      </c>
-      <c r="T36" t="inlineStr">
-        <is>
-          <t>Short</t>
-        </is>
-      </c>
-      <c r="U36" t="n">
         <v>-1225</v>
       </c>
     </row>
@@ -3425,7 +3350,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.1599</v>
+        <v>1.1645</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -3455,17 +3380,17 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M2" t="n">
         <v>1000</v>
       </c>
       <c r="N2" t="n">
-        <v>47.82</v>
+        <v>46.44</v>
       </c>
       <c r="O2" t="n">
-        <v>47820</v>
+        <v>46440</v>
       </c>
       <c r="P2" t="n">
         <v>43.01</v>
@@ -3477,7 +3402,7 @@
         <v>43010</v>
       </c>
       <c r="S2" t="n">
-        <v>4810</v>
+        <v>3430</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -3485,7 +3410,7 @@
         </is>
       </c>
       <c r="U2" t="n">
-        <v>55466.418</v>
+        <v>54079.38</v>
       </c>
     </row>
     <row r="3">
@@ -3500,7 +3425,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.1599</v>
+        <v>1.1645</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -3530,29 +3455,29 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N3" t="n">
-        <v>609.2</v>
+        <v>582.8</v>
       </c>
       <c r="O3" t="n">
-        <v>6092</v>
+        <v>2914</v>
       </c>
       <c r="P3" t="n">
-        <v>624.2</v>
+        <v>624.1</v>
       </c>
       <c r="Q3" t="n">
-        <v>624.2</v>
+        <v>624.1</v>
       </c>
       <c r="R3" t="n">
-        <v>6242</v>
+        <v>3120.5</v>
       </c>
       <c r="S3" t="n">
-        <v>-150</v>
+        <v>-206.5</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
@@ -3560,7 +3485,7 @@
         </is>
       </c>
       <c r="U3" t="n">
-        <v>7066.110799999999</v>
+        <v>3393.353</v>
       </c>
     </row>
     <row r="4">
@@ -3575,7 +3500,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.1599</v>
+        <v>1.1645</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -3605,17 +3530,17 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M4" t="n">
         <v>3</v>
       </c>
       <c r="N4" t="n">
-        <v>2190</v>
+        <v>2113</v>
       </c>
       <c r="O4" t="n">
-        <v>6570</v>
+        <v>6339</v>
       </c>
       <c r="P4" t="n">
         <v>2127.063</v>
@@ -3627,7 +3552,7 @@
         <v>6381.189</v>
       </c>
       <c r="S4" t="n">
-        <v>188.811</v>
+        <v>-42.189</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
@@ -3635,7 +3560,7 @@
         </is>
       </c>
       <c r="U4" t="n">
-        <v>7620.543</v>
+        <v>7381.7655</v>
       </c>
     </row>
     <row r="5">
@@ -3650,7 +3575,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.1599</v>
+        <v>1.1645</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -3680,17 +3605,17 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M5" t="n">
         <v>400</v>
       </c>
       <c r="N5" t="n">
-        <v>149.9</v>
+        <v>148.04</v>
       </c>
       <c r="O5" t="n">
-        <v>59960</v>
+        <v>59216</v>
       </c>
       <c r="P5" t="n">
         <v>146.3403336</v>
@@ -3702,7 +3627,7 @@
         <v>58536.13344</v>
       </c>
       <c r="S5" t="n">
-        <v>1423.86656</v>
+        <v>679.86656</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -3710,7 +3635,7 @@
         </is>
       </c>
       <c r="U5" t="n">
-        <v>69547.60399999999</v>
+        <v>68957.03200000001</v>
       </c>
     </row>
     <row r="6">
@@ -3725,7 +3650,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.77579</v>
+        <v>0.77833</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -3755,17 +3680,17 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M6" t="n">
         <v>10000</v>
       </c>
       <c r="N6" t="n">
-        <v>4.927</v>
+        <v>4.905</v>
       </c>
       <c r="O6" t="n">
-        <v>49270</v>
+        <v>49050</v>
       </c>
       <c r="P6" t="n">
         <v>3.81181816</v>
@@ -3777,7 +3702,7 @@
         <v>38118.1816</v>
       </c>
       <c r="S6" t="n">
-        <v>11151.8184</v>
+        <v>10931.8184</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
@@ -3785,7 +3710,7 @@
         </is>
       </c>
       <c r="U6" t="n">
-        <v>38223.1733</v>
+        <v>38177.0865</v>
       </c>
     </row>
     <row r="7">
@@ -3800,7 +3725,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.77579</v>
+        <v>0.77833</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -3830,17 +3755,17 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M7" t="n">
         <v>10</v>
       </c>
       <c r="N7" t="n">
-        <v>545.45</v>
+        <v>552.1</v>
       </c>
       <c r="O7" t="n">
-        <v>5454.5</v>
+        <v>5521</v>
       </c>
       <c r="P7" t="n">
         <v>544.755456</v>
@@ -3852,7 +3777,7 @@
         <v>5447.55456</v>
       </c>
       <c r="S7" t="n">
-        <v>6.94544</v>
+        <v>73.44544</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -3860,7 +3785,7 @@
         </is>
       </c>
       <c r="U7" t="n">
-        <v>4231.546555</v>
+        <v>4297.15993</v>
       </c>
     </row>
     <row r="8">
@@ -3905,7 +3830,7 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -3980,17 +3905,17 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M9" t="n">
         <v>15</v>
       </c>
       <c r="N9" t="n">
-        <v>1468</v>
+        <v>1444</v>
       </c>
       <c r="O9" t="n">
-        <v>22020</v>
+        <v>21660</v>
       </c>
       <c r="P9" t="n">
         <v>1461.150733333</v>
@@ -4002,7 +3927,7 @@
         <v>21917.261</v>
       </c>
       <c r="S9" t="n">
-        <v>102.739</v>
+        <v>-257.261</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -4010,7 +3935,7 @@
         </is>
       </c>
       <c r="U9" t="n">
-        <v>22020</v>
+        <v>21660</v>
       </c>
     </row>
     <row r="10">
@@ -4055,17 +3980,17 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M10" t="n">
         <v>3000</v>
       </c>
       <c r="N10" t="n">
-        <v>5.473</v>
+        <v>5.488</v>
       </c>
       <c r="O10" t="n">
-        <v>16419</v>
+        <v>16464</v>
       </c>
       <c r="P10" t="n">
         <v>5.552814967</v>
@@ -4077,7 +4002,7 @@
         <v>16658.4449</v>
       </c>
       <c r="S10" t="n">
-        <v>-239.4449</v>
+        <v>-194.4449</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -4085,7 +4010,7 @@
         </is>
       </c>
       <c r="U10" t="n">
-        <v>16419</v>
+        <v>16464</v>
       </c>
     </row>
     <row r="11">
@@ -4130,17 +4055,17 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M11" t="n">
         <v>1000</v>
       </c>
       <c r="N11" t="n">
-        <v>9.42</v>
+        <v>9.2675</v>
       </c>
       <c r="O11" t="n">
-        <v>9420</v>
+        <v>9267.5</v>
       </c>
       <c r="P11" t="n">
         <v>9.405900600000001</v>
@@ -4152,7 +4077,7 @@
         <v>9405.900600000001</v>
       </c>
       <c r="S11" t="n">
-        <v>14.0994</v>
+        <v>-138.4006</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -4160,7 +4085,7 @@
         </is>
       </c>
       <c r="U11" t="n">
-        <v>9420</v>
+        <v>9267.5</v>
       </c>
     </row>
     <row r="12">
@@ -4205,7 +4130,7 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M12" t="n">
@@ -4280,17 +4205,17 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M13" t="n">
         <v>385</v>
       </c>
       <c r="N13" t="n">
-        <v>26.1068</v>
+        <v>25.9392</v>
       </c>
       <c r="O13" t="n">
-        <v>10051.12</v>
+        <v>9986.59</v>
       </c>
       <c r="P13" t="n">
         <v>25.997158151</v>
@@ -4302,7 +4227,7 @@
         <v>10008.905888</v>
       </c>
       <c r="S13" t="n">
-        <v>42.214112</v>
+        <v>-22.315888</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -4310,7 +4235,7 @@
         </is>
       </c>
       <c r="U13" t="n">
-        <v>10051.12</v>
+        <v>9986.59</v>
       </c>
     </row>
     <row r="14">
@@ -4355,7 +4280,7 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M14" t="n">
@@ -4430,17 +4355,17 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M15" t="n">
         <v>1000</v>
       </c>
       <c r="N15" t="n">
-        <v>10.127</v>
+        <v>9.939</v>
       </c>
       <c r="O15" t="n">
-        <v>10127</v>
+        <v>9939</v>
       </c>
       <c r="P15" t="n">
         <v>10.229112</v>
@@ -4452,7 +4377,7 @@
         <v>10229.112</v>
       </c>
       <c r="S15" t="n">
-        <v>-102.112</v>
+        <v>-290.112</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -4460,7 +4385,7 @@
         </is>
       </c>
       <c r="U15" t="n">
-        <v>10127</v>
+        <v>9939</v>
       </c>
     </row>
     <row r="16">
@@ -4505,17 +4430,17 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M16" t="n">
         <v>800</v>
       </c>
       <c r="N16" t="n">
-        <v>173.84</v>
+        <v>172.46</v>
       </c>
       <c r="O16" t="n">
-        <v>139072</v>
+        <v>137968</v>
       </c>
       <c r="P16" t="n">
         <v>170.683661681</v>
@@ -4527,7 +4452,7 @@
         <v>136546.929345</v>
       </c>
       <c r="S16" t="n">
-        <v>2525.070655</v>
+        <v>1421.070655</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
@@ -4535,7 +4460,7 @@
         </is>
       </c>
       <c r="U16" t="n">
-        <v>139072</v>
+        <v>137968</v>
       </c>
     </row>
     <row r="17">
@@ -4590,7 +4515,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M17" t="n">
@@ -4675,7 +4600,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M18" t="n">
@@ -4760,7 +4685,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M19" t="n">
@@ -4845,7 +4770,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="M20" t="n">
@@ -4927,11 +4852,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-20 10:55:19</t>
+          <t>2026-01-20 23:31:44</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="n">
         <v>19</v>

</xml_diff>

<commit_message>
Add Portfolio Risk Analyzer for VaR & CVaR calculations
- Implemented a comprehensive portfolio risk analysis tool in `portfolio-risk-var-cvar.py` to calculate Value at Risk (VaR) and Conditional VaR (CVaR) for IBKR portfolio positions.
- Included methods for historical, parametric, and Monte Carlo simulations for risk assessment.
- Integrated Telegram alerts for daily risk summaries.
- Added functionality to load positions from an Excel file and fetch historical price data using yfinance.
- Calculated individual position contributions to overall portfolio risk.
- Saved results in a JSON file format for easy access and review.
- Created a sample JSON output file `portfolio_risk_20260125.json` to demonstrate the results structure.
- Added a temporary Excel file `fetch-ibkr-positions-dashboard.xlsx` for position data.
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions.xlsx
+++ b/projects/fetch-ibkr-positions.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PositionsHK" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PositionsAL" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metadata" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metadata" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,6 +539,11 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
+          <t>ListingExchange</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
           <t>PositionValueUSD</t>
         </is>
       </c>
@@ -554,7 +560,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.14369</v>
+        <v>0.14391</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -584,17 +590,17 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M2" t="n">
         <v>1000</v>
       </c>
       <c r="N2" t="n">
-        <v>31.66</v>
+        <v>31.56</v>
       </c>
       <c r="O2" t="n">
-        <v>31660</v>
+        <v>31560</v>
       </c>
       <c r="P2" t="n">
         <v>30.68540181</v>
@@ -606,15 +612,20 @@
         <v>30685.40181</v>
       </c>
       <c r="S2" t="n">
-        <v>974.59819</v>
+        <v>874.59819</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U2" t="n">
-        <v>4549.2254</v>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>SEHK</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>4541.7996</v>
       </c>
     </row>
     <row r="3">
@@ -629,7 +640,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.1686</v>
+        <v>1.1828</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -659,17 +670,17 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M3" t="n">
         <v>3</v>
       </c>
       <c r="N3" t="n">
-        <v>2098</v>
+        <v>2130</v>
       </c>
       <c r="O3" t="n">
-        <v>6294</v>
+        <v>6390</v>
       </c>
       <c r="P3" t="n">
         <v>2126.0625</v>
@@ -681,15 +692,20 @@
         <v>6378.1875</v>
       </c>
       <c r="S3" t="n">
-        <v>-84.1875</v>
+        <v>11.8125</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U3" t="n">
-        <v>7355.1684</v>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>SBF</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>7558.092000000001</v>
       </c>
     </row>
     <row r="4">
@@ -704,7 +720,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.77847</v>
+        <v>0.7861900000000001</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -734,17 +750,17 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M4" t="n">
         <v>5000</v>
       </c>
       <c r="N4" t="n">
-        <v>4.888</v>
+        <v>4.97</v>
       </c>
       <c r="O4" t="n">
-        <v>24440</v>
+        <v>24850</v>
       </c>
       <c r="P4" t="n">
         <v>4.54124249</v>
@@ -756,15 +772,20 @@
         <v>22706.21245</v>
       </c>
       <c r="S4" t="n">
-        <v>1733.78755</v>
+        <v>2143.78755</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U4" t="n">
-        <v>19025.8068</v>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>SGX</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>19536.8215</v>
       </c>
     </row>
     <row r="5">
@@ -779,7 +800,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.77847</v>
+        <v>0.7861900000000001</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -809,17 +830,17 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M5" t="n">
         <v>50</v>
       </c>
       <c r="N5" t="n">
-        <v>574.1</v>
+        <v>577.5</v>
       </c>
       <c r="O5" t="n">
-        <v>28705</v>
+        <v>28875</v>
       </c>
       <c r="P5" t="n">
         <v>432.4596912</v>
@@ -831,15 +852,20 @@
         <v>21622.98456</v>
       </c>
       <c r="S5" t="n">
-        <v>7082.01544</v>
+        <v>7252.01544</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U5" t="n">
-        <v>22345.98135</v>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>SGX</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>22701.23625</v>
       </c>
     </row>
     <row r="6">
@@ -884,17 +910,17 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M6" t="n">
         <v>100</v>
       </c>
       <c r="N6" t="n">
-        <v>231.31</v>
+        <v>239.16</v>
       </c>
       <c r="O6" t="n">
-        <v>23131</v>
+        <v>23916</v>
       </c>
       <c r="P6" t="n">
         <v>216.590322</v>
@@ -906,15 +932,20 @@
         <v>21659.0322</v>
       </c>
       <c r="S6" t="n">
-        <v>1471.9678</v>
+        <v>2256.9678</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U6" t="n">
-        <v>23131</v>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>23916</v>
       </c>
     </row>
     <row r="7">
@@ -959,17 +990,17 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M7" t="n">
         <v>100</v>
       </c>
       <c r="N7" t="n">
-        <v>12.49</v>
+        <v>12.4</v>
       </c>
       <c r="O7" t="n">
-        <v>1249</v>
+        <v>1240</v>
       </c>
       <c r="P7" t="n">
         <v>12.97</v>
@@ -981,15 +1012,20 @@
         <v>1297</v>
       </c>
       <c r="S7" t="n">
-        <v>-48</v>
+        <v>-57</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U7" t="n">
-        <v>1249</v>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>ARCA</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>1240</v>
       </c>
     </row>
     <row r="8">
@@ -1034,17 +1070,17 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M8" t="n">
         <v>50</v>
       </c>
       <c r="N8" t="n">
-        <v>56.44</v>
+        <v>55.94</v>
       </c>
       <c r="O8" t="n">
-        <v>2822</v>
+        <v>2797</v>
       </c>
       <c r="P8" t="n">
         <v>46.285022</v>
@@ -1056,15 +1092,20 @@
         <v>2314.2511</v>
       </c>
       <c r="S8" t="n">
-        <v>507.7489</v>
+        <v>482.7489</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U8" t="n">
-        <v>2822</v>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>2797</v>
       </c>
     </row>
     <row r="9">
@@ -1109,17 +1150,17 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M9" t="n">
         <v>100</v>
       </c>
       <c r="N9" t="n">
-        <v>11.9</v>
+        <v>12.27</v>
       </c>
       <c r="O9" t="n">
-        <v>1190</v>
+        <v>1227</v>
       </c>
       <c r="P9" t="n">
         <v>12.49</v>
@@ -1131,15 +1172,20 @@
         <v>1249</v>
       </c>
       <c r="S9" t="n">
-        <v>-59</v>
+        <v>-22</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U9" t="n">
-        <v>1190</v>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V9" t="n">
+        <v>1227</v>
       </c>
     </row>
     <row r="10">
@@ -1184,37 +1230,42 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N10" t="n">
-        <v>1448.2</v>
+        <v>1470.8</v>
       </c>
       <c r="O10" t="n">
-        <v>14482</v>
+        <v>22062</v>
       </c>
       <c r="P10" t="n">
-        <v>1476.8770695</v>
+        <v>1472.214713</v>
       </c>
       <c r="Q10" t="n">
-        <v>1476.8770695</v>
+        <v>1472.214713</v>
       </c>
       <c r="R10" t="n">
-        <v>14768.770695</v>
+        <v>22083.220695</v>
       </c>
       <c r="S10" t="n">
-        <v>-286.770695</v>
+        <v>-21.220695</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U10" t="n">
-        <v>14482</v>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>EBS</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>22062</v>
       </c>
     </row>
     <row r="11">
@@ -1259,17 +1310,17 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M11" t="n">
         <v>2000</v>
       </c>
       <c r="N11" t="n">
-        <v>5.481</v>
+        <v>5.526</v>
       </c>
       <c r="O11" t="n">
-        <v>10962</v>
+        <v>11052</v>
       </c>
       <c r="P11" t="n">
         <v>5.5697835</v>
@@ -1281,15 +1332,20 @@
         <v>11139.567</v>
       </c>
       <c r="S11" t="n">
-        <v>-177.567</v>
+        <v>-87.56699999999999</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U11" t="n">
-        <v>10962</v>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>EBS</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v>11052</v>
       </c>
     </row>
     <row r="12">
@@ -1334,17 +1390,17 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M12" t="n">
         <v>100</v>
       </c>
       <c r="N12" t="n">
-        <v>328.38</v>
+        <v>327.93</v>
       </c>
       <c r="O12" t="n">
-        <v>32838</v>
+        <v>32793</v>
       </c>
       <c r="P12" t="n">
         <v>312.15</v>
@@ -1356,15 +1412,20 @@
         <v>31215</v>
       </c>
       <c r="S12" t="n">
-        <v>1623</v>
+        <v>1578</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U12" t="n">
-        <v>32838</v>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V12" t="n">
+        <v>32793</v>
       </c>
     </row>
     <row r="13">
@@ -1409,17 +1470,17 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M13" t="n">
         <v>500</v>
       </c>
       <c r="N13" t="n">
-        <v>4.4</v>
+        <v>4.58</v>
       </c>
       <c r="O13" t="n">
-        <v>2200</v>
+        <v>2290</v>
       </c>
       <c r="P13" t="n">
         <v>5.166</v>
@@ -1431,15 +1492,20 @@
         <v>2583</v>
       </c>
       <c r="S13" t="n">
-        <v>-383</v>
+        <v>-293</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U13" t="n">
-        <v>2200</v>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V13" t="n">
+        <v>2290</v>
       </c>
     </row>
     <row r="14">
@@ -1484,17 +1550,17 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M14" t="n">
         <v>1000</v>
       </c>
       <c r="N14" t="n">
-        <v>9.43</v>
+        <v>9.494999999999999</v>
       </c>
       <c r="O14" t="n">
-        <v>9430</v>
+        <v>9495</v>
       </c>
       <c r="P14" t="n">
         <v>9.424709999999999</v>
@@ -1506,15 +1572,20 @@
         <v>9424.709999999999</v>
       </c>
       <c r="S14" t="n">
-        <v>5.29</v>
+        <v>70.29000000000001</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U14" t="n">
-        <v>9430</v>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>LSEETF</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>9495</v>
       </c>
     </row>
     <row r="15">
@@ -1559,17 +1630,17 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M15" t="n">
         <v>385</v>
       </c>
       <c r="N15" t="n">
-        <v>26.0432</v>
+        <v>27.0092</v>
       </c>
       <c r="O15" t="n">
-        <v>10026.63</v>
+        <v>10398.54</v>
       </c>
       <c r="P15" t="n">
         <v>26.012734603</v>
@@ -1581,15 +1652,20 @@
         <v>10014.902822</v>
       </c>
       <c r="S15" t="n">
-        <v>11.727178</v>
+        <v>383.637178</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U15" t="n">
-        <v>10026.63</v>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>AEB</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>10398.54</v>
       </c>
     </row>
     <row r="16">
@@ -1634,17 +1710,17 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M16" t="n">
         <v>50</v>
       </c>
       <c r="N16" t="n">
-        <v>33.25</v>
+        <v>33.42</v>
       </c>
       <c r="O16" t="n">
-        <v>1662.5</v>
+        <v>1671</v>
       </c>
       <c r="P16" t="n">
         <v>36.96000022</v>
@@ -1656,15 +1732,20 @@
         <v>1848.000011</v>
       </c>
       <c r="S16" t="n">
-        <v>-185.500011</v>
+        <v>-177.000011</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U16" t="n">
-        <v>1662.5</v>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>PINK</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
+        <v>1671</v>
       </c>
     </row>
     <row r="17">
@@ -1709,17 +1790,17 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M17" t="n">
         <v>1000</v>
       </c>
       <c r="N17" t="n">
-        <v>9.952</v>
+        <v>10.02</v>
       </c>
       <c r="O17" t="n">
-        <v>9952</v>
+        <v>10020</v>
       </c>
       <c r="P17" t="n">
         <v>10.2267108</v>
@@ -1731,15 +1812,20 @@
         <v>10226.7108</v>
       </c>
       <c r="S17" t="n">
-        <v>-274.7108</v>
+        <v>-206.7108</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U17" t="n">
-        <v>9952</v>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>LSEETF</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
+        <v>10020</v>
       </c>
     </row>
     <row r="18">
@@ -1784,17 +1870,17 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M18" t="n">
         <v>1</v>
       </c>
       <c r="N18" t="n">
-        <v>2057.77</v>
+        <v>2137.29</v>
       </c>
       <c r="O18" t="n">
-        <v>2057.77</v>
+        <v>2137.29</v>
       </c>
       <c r="P18" t="n">
         <v>2086.200022</v>
@@ -1806,15 +1892,20 @@
         <v>2086.200022</v>
       </c>
       <c r="S18" t="n">
-        <v>-28.430022</v>
+        <v>51.089978</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U18" t="n">
-        <v>2057.77</v>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V18" t="n">
+        <v>2137.29</v>
       </c>
     </row>
     <row r="19">
@@ -1859,17 +1950,17 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M19" t="n">
         <v>200</v>
       </c>
       <c r="N19" t="n">
-        <v>183.32</v>
+        <v>187.67</v>
       </c>
       <c r="O19" t="n">
-        <v>36664</v>
+        <v>37534</v>
       </c>
       <c r="P19" t="n">
         <v>185.216422</v>
@@ -1881,15 +1972,20 @@
         <v>37043.2844</v>
       </c>
       <c r="S19" t="n">
-        <v>-379.2844</v>
+        <v>490.7156</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U19" t="n">
-        <v>36664</v>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V19" t="n">
+        <v>37534</v>
       </c>
     </row>
     <row r="20">
@@ -1934,17 +2030,17 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M20" t="n">
         <v>100</v>
       </c>
       <c r="N20" t="n">
-        <v>173.88</v>
+        <v>177.16</v>
       </c>
       <c r="O20" t="n">
-        <v>17388</v>
+        <v>17716</v>
       </c>
       <c r="P20" t="n">
         <v>205.3357044</v>
@@ -1956,15 +2052,20 @@
         <v>20533.57044</v>
       </c>
       <c r="S20" t="n">
-        <v>-3145.57044</v>
+        <v>-2817.57044</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U20" t="n">
-        <v>17388</v>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="V20" t="n">
+        <v>17716</v>
       </c>
     </row>
     <row r="21">
@@ -2009,17 +2110,17 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M21" t="n">
         <v>10</v>
       </c>
       <c r="N21" t="n">
-        <v>121.13</v>
+        <v>124.78</v>
       </c>
       <c r="O21" t="n">
-        <v>1211.3</v>
+        <v>1247.8</v>
       </c>
       <c r="P21" t="n">
         <v>128.6</v>
@@ -2031,15 +2132,20 @@
         <v>1286</v>
       </c>
       <c r="S21" t="n">
-        <v>-74.7</v>
+        <v>-38.2</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U21" t="n">
-        <v>1211.3</v>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="V21" t="n">
+        <v>1247.8</v>
       </c>
     </row>
     <row r="22">
@@ -2084,17 +2190,17 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M22" t="n">
         <v>600</v>
       </c>
       <c r="N22" t="n">
-        <v>172.18</v>
+        <v>173.74</v>
       </c>
       <c r="O22" t="n">
-        <v>103308</v>
+        <v>104244</v>
       </c>
       <c r="P22" t="n">
         <v>170.213547575</v>
@@ -2106,15 +2212,20 @@
         <v>102128.128545</v>
       </c>
       <c r="S22" t="n">
-        <v>1179.871455</v>
+        <v>2115.871455</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U22" t="n">
-        <v>103308</v>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>LSEETF</t>
+        </is>
+      </c>
+      <c r="V22" t="n">
+        <v>104244</v>
       </c>
     </row>
     <row r="23">
@@ -2143,23 +2254,23 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>QQQ   260220P00605000</t>
+          <t>JPM   260206P00320000</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>QQQ 20FEB26 605 P</t>
+          <t>JPM 06FEB26 320 P</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>100</v>
       </c>
       <c r="I23" t="n">
-        <v>605</v>
+        <v>320</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2169,37 +2280,42 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M23" t="n">
         <v>1</v>
       </c>
       <c r="N23" t="n">
-        <v>8.945</v>
+        <v>22.3276</v>
       </c>
       <c r="O23" t="n">
-        <v>894.5</v>
+        <v>2232.76</v>
       </c>
       <c r="P23" t="n">
-        <v>11.0485875</v>
+        <v>21.7804875</v>
       </c>
       <c r="Q23" t="n">
-        <v>11.0485875</v>
+        <v>21.7804875</v>
       </c>
       <c r="R23" t="n">
-        <v>1104.85875</v>
+        <v>2178.04875</v>
       </c>
       <c r="S23" t="n">
-        <v>-210.35875</v>
+        <v>54.71125</v>
       </c>
       <c r="T23" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U23" t="n">
-        <v>894.5</v>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V23" t="n">
+        <v>2232.76</v>
       </c>
     </row>
     <row r="24">
@@ -2218,7 +2334,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>FOP</t>
+          <t>OPT</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2228,23 +2344,23 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>EW2G6 P6525</t>
+          <t>QQQ   260220P00605000</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>ES 13FEB26 6525 P</t>
+          <t>QQQ 20FEB26 605 P</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I24" t="n">
-        <v>6525</v>
+        <v>605</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2254,37 +2370,42 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N24" t="n">
-        <v>22.5</v>
+        <v>6.34</v>
       </c>
       <c r="O24" t="n">
-        <v>2250</v>
+        <v>634</v>
       </c>
       <c r="P24" t="n">
-        <v>31.5284</v>
+        <v>11.0485875</v>
       </c>
       <c r="Q24" t="n">
-        <v>31.5284</v>
+        <v>11.0485875</v>
       </c>
       <c r="R24" t="n">
-        <v>3152.84</v>
+        <v>1104.85875</v>
       </c>
       <c r="S24" t="n">
-        <v>-902.84</v>
+        <v>-470.85875</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U24" t="n">
-        <v>2250</v>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V24" t="n">
+        <v>634</v>
       </c>
     </row>
     <row r="25">
@@ -2308,24 +2429,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>EW2G6 C7300</t>
+          <t>EW2G6 P6525</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>ES 13FEB26 7300 C</t>
+          <t>ES 13FEB26 6525 P</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>50</v>
       </c>
       <c r="I25" t="n">
-        <v>7300</v>
+        <v>6525</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2334,42 +2455,47 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M25" t="n">
         <v>2</v>
       </c>
       <c r="N25" t="n">
-        <v>1.5</v>
+        <v>13.75</v>
       </c>
       <c r="O25" t="n">
-        <v>150</v>
+        <v>1375</v>
       </c>
       <c r="P25" t="n">
-        <v>8.0284</v>
+        <v>31.5284</v>
       </c>
       <c r="Q25" t="n">
-        <v>8.0284</v>
+        <v>31.5284</v>
       </c>
       <c r="R25" t="n">
-        <v>802.84</v>
+        <v>3152.84</v>
       </c>
       <c r="S25" t="n">
-        <v>-652.84</v>
+        <v>-1777.84</v>
       </c>
       <c r="T25" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U25" t="n">
-        <v>150</v>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>CME</t>
+        </is>
+      </c>
+      <c r="V25" t="n">
+        <v>1375</v>
       </c>
     </row>
     <row r="26">
@@ -2388,73 +2514,78 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>OPT</t>
+          <t>FOP</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>AMZN  260220P00215000</t>
+          <t>EW2G6 C7300</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>AMZN 20FEB26 215 P</t>
+          <t>ES 13FEB26 7300 C</t>
         </is>
       </c>
       <c r="H26" t="n">
+        <v>50</v>
+      </c>
+      <c r="I26" t="n">
+        <v>7300</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>2</v>
+      </c>
+      <c r="N26" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" t="n">
         <v>100</v>
       </c>
-      <c r="I26" t="n">
-        <v>215</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>2026-02-20</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>2026-01-21</t>
-        </is>
-      </c>
-      <c r="M26" t="n">
-        <v>-1</v>
-      </c>
-      <c r="N26" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="O26" t="n">
-        <v>-420</v>
-      </c>
       <c r="P26" t="n">
-        <v>4.3794796</v>
+        <v>8.0284</v>
       </c>
       <c r="Q26" t="n">
-        <v>4.3794796</v>
+        <v>8.0284</v>
       </c>
       <c r="R26" t="n">
-        <v>-437.94796</v>
+        <v>802.84</v>
       </c>
       <c r="S26" t="n">
-        <v>17.94796</v>
+        <v>-702.84</v>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>Short</t>
-        </is>
-      </c>
-      <c r="U26" t="n">
-        <v>-420</v>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>CME</t>
+        </is>
+      </c>
+      <c r="V26" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="27">
@@ -2478,68 +2609,73 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>AMZN  260227C00255000</t>
+          <t>AMZN  260220P00215000</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>AMZN 27FEB26 255 C</t>
+          <t>AMZN 20FEB26 215 P</t>
         </is>
       </c>
       <c r="H27" t="n">
         <v>100</v>
       </c>
       <c r="I27" t="n">
-        <v>255</v>
+        <v>215</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2026-02-27</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M27" t="n">
         <v>-1</v>
       </c>
       <c r="N27" t="n">
-        <v>3.35</v>
+        <v>2.605</v>
       </c>
       <c r="O27" t="n">
-        <v>-335</v>
+        <v>-260.5</v>
       </c>
       <c r="P27" t="n">
-        <v>5.4294796</v>
+        <v>4.3794796</v>
       </c>
       <c r="Q27" t="n">
-        <v>5.4294796</v>
+        <v>4.3794796</v>
       </c>
       <c r="R27" t="n">
-        <v>-542.94796</v>
+        <v>-437.94796</v>
       </c>
       <c r="S27" t="n">
-        <v>207.94796</v>
+        <v>177.44796</v>
       </c>
       <c r="T27" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U27" t="n">
-        <v>-335</v>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V27" t="n">
+        <v>-260.5</v>
       </c>
     </row>
     <row r="28">
@@ -2563,24 +2699,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>GOOGL 260227P00310000</t>
+          <t>AMZN  260227C00255000</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>GOOGL 27FEB26 310 P</t>
+          <t>AMZN 27FEB26 255 C</t>
         </is>
       </c>
       <c r="H28" t="n">
         <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>310</v>
+        <v>255</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2589,42 +2725,47 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M28" t="n">
         <v>-1</v>
       </c>
       <c r="N28" t="n">
-        <v>7.225</v>
+        <v>5.4994</v>
       </c>
       <c r="O28" t="n">
-        <v>-722.5</v>
+        <v>-549.9400000000001</v>
       </c>
       <c r="P28" t="n">
-        <v>7.2294546</v>
+        <v>5.4294796</v>
       </c>
       <c r="Q28" t="n">
-        <v>7.2294546</v>
+        <v>5.4294796</v>
       </c>
       <c r="R28" t="n">
-        <v>-722.94546</v>
+        <v>-542.94796</v>
       </c>
       <c r="S28" t="n">
-        <v>0.44546</v>
+        <v>-6.99204</v>
       </c>
       <c r="T28" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U28" t="n">
-        <v>-722.5</v>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V28" t="n">
+        <v>-549.9400000000001</v>
       </c>
     </row>
     <row r="29">
@@ -2648,24 +2789,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>GOOGL 260227C00370000</t>
+          <t>GOOGL 260227P00310000</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>GOOGL 27FEB26 370 C</t>
+          <t>GOOGL 27FEB26 310 P</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>100</v>
       </c>
       <c r="I29" t="n">
-        <v>370</v>
+        <v>310</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2674,42 +2815,47 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M29" t="n">
         <v>-1</v>
       </c>
       <c r="N29" t="n">
-        <v>3.05</v>
+        <v>6.975</v>
       </c>
       <c r="O29" t="n">
-        <v>-305</v>
+        <v>-697.5</v>
       </c>
       <c r="P29" t="n">
-        <v>5.6494546</v>
+        <v>7.2294546</v>
       </c>
       <c r="Q29" t="n">
-        <v>5.6494546</v>
+        <v>7.2294546</v>
       </c>
       <c r="R29" t="n">
-        <v>-564.94546</v>
+        <v>-722.94546</v>
       </c>
       <c r="S29" t="n">
-        <v>259.94546</v>
+        <v>25.44546</v>
       </c>
       <c r="T29" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U29" t="n">
-        <v>-305</v>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V29" t="n">
+        <v>-697.5</v>
       </c>
     </row>
     <row r="30">
@@ -2733,68 +2879,73 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>JPM   260206P00300000</t>
+          <t>GOOGL 260227C00370000</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>JPM 06FEB26 300 P</t>
+          <t>GOOGL 27FEB26 370 C</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>100</v>
       </c>
       <c r="I30" t="n">
-        <v>300</v>
+        <v>370</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-27</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M30" t="n">
         <v>-1</v>
       </c>
       <c r="N30" t="n">
-        <v>4.5529</v>
+        <v>2.78</v>
       </c>
       <c r="O30" t="n">
-        <v>-455.29</v>
+        <v>-278</v>
       </c>
       <c r="P30" t="n">
-        <v>2.4194546</v>
+        <v>5.6494546</v>
       </c>
       <c r="Q30" t="n">
-        <v>2.4194546</v>
+        <v>5.6494546</v>
       </c>
       <c r="R30" t="n">
-        <v>-241.94546</v>
+        <v>-564.94546</v>
       </c>
       <c r="S30" t="n">
-        <v>-213.34454</v>
+        <v>286.94546</v>
       </c>
       <c r="T30" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U30" t="n">
-        <v>-455.29</v>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V30" t="n">
+        <v>-278</v>
       </c>
     </row>
     <row r="31">
@@ -2818,68 +2969,73 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>NVDA  260130C00195000</t>
+          <t>JPM   260206P00300000</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>NVDA 30JAN26 195 C</t>
+          <t>JPM 06FEB26 300 P</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>195</v>
+        <v>300</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="N31" t="n">
-        <v>0.82</v>
+        <v>6.0792</v>
       </c>
       <c r="O31" t="n">
-        <v>-164</v>
+        <v>-607.92</v>
       </c>
       <c r="P31" t="n">
-        <v>2.1886796</v>
+        <v>2.4194546</v>
       </c>
       <c r="Q31" t="n">
-        <v>2.1886796</v>
+        <v>2.4194546</v>
       </c>
       <c r="R31" t="n">
-        <v>-437.73592</v>
+        <v>-241.94546</v>
       </c>
       <c r="S31" t="n">
-        <v>273.73592</v>
+        <v>-365.97454</v>
       </c>
       <c r="T31" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U31" t="n">
-        <v>-164</v>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V31" t="n">
+        <v>-607.92</v>
       </c>
     </row>
     <row r="32">
@@ -2908,23 +3064,23 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>ORCL  260220C00200000</t>
+          <t>NVDA  260130C00195000</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>ORCL 20FEB26 200 C</t>
+          <t>NVDA 30JAN26 195 C</t>
         </is>
       </c>
       <c r="H32" t="n">
         <v>100</v>
       </c>
       <c r="I32" t="n">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2934,37 +3090,42 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N32" t="n">
-        <v>2.2</v>
+        <v>1.115</v>
       </c>
       <c r="O32" t="n">
-        <v>-220</v>
+        <v>-223</v>
       </c>
       <c r="P32" t="n">
-        <v>2.3894796</v>
+        <v>2.1886796</v>
       </c>
       <c r="Q32" t="n">
-        <v>2.3894796</v>
+        <v>2.1886796</v>
       </c>
       <c r="R32" t="n">
-        <v>-238.94796</v>
+        <v>-437.73592</v>
       </c>
       <c r="S32" t="n">
-        <v>18.94796</v>
+        <v>214.73592</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U32" t="n">
-        <v>-220</v>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V32" t="n">
+        <v>-223</v>
       </c>
     </row>
     <row r="33">
@@ -2988,24 +3149,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>QQQ   260220P00570000</t>
+          <t>ORCL  260220C00200000</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>QQQ 20FEB26 570 P</t>
+          <t>ORCL 20FEB26 200 C</t>
         </is>
       </c>
       <c r="H33" t="n">
         <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>570</v>
+        <v>200</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3014,42 +3175,47 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M33" t="n">
         <v>-1</v>
       </c>
       <c r="N33" t="n">
-        <v>2.995</v>
+        <v>2.365</v>
       </c>
       <c r="O33" t="n">
-        <v>-299.5</v>
+        <v>-236.5</v>
       </c>
       <c r="P33" t="n">
-        <v>3.8813796</v>
+        <v>2.3894796</v>
       </c>
       <c r="Q33" t="n">
-        <v>3.8813796</v>
+        <v>2.3894796</v>
       </c>
       <c r="R33" t="n">
-        <v>-388.13796</v>
+        <v>-238.94796</v>
       </c>
       <c r="S33" t="n">
-        <v>88.63796000000001</v>
+        <v>2.44796</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U33" t="n">
-        <v>-299.5</v>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V33" t="n">
+        <v>-236.5</v>
       </c>
     </row>
     <row r="34">
@@ -3068,7 +3234,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>FOP</t>
+          <t>OPT</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -3078,23 +3244,23 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>EW2G6 P6625</t>
+          <t>QQQ   260220P00570000</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>ES 13FEB26 6625 P</t>
+          <t>QQQ 20FEB26 570 P</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I34" t="n">
-        <v>6625</v>
+        <v>570</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -3104,37 +3270,42 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="N34" t="n">
-        <v>32.5</v>
+        <v>1.895</v>
       </c>
       <c r="O34" t="n">
-        <v>-3250</v>
+        <v>-189.5</v>
       </c>
       <c r="P34" t="n">
-        <v>42.2216</v>
+        <v>3.8813796</v>
       </c>
       <c r="Q34" t="n">
-        <v>42.2216</v>
+        <v>3.8813796</v>
       </c>
       <c r="R34" t="n">
-        <v>-4222.16</v>
+        <v>-388.13796</v>
       </c>
       <c r="S34" t="n">
-        <v>972.16</v>
+        <v>198.63796</v>
       </c>
       <c r="T34" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U34" t="n">
-        <v>-3250</v>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V34" t="n">
+        <v>-189.5</v>
       </c>
     </row>
     <row r="35">
@@ -3158,24 +3329,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>EW2G6 C7200</t>
+          <t>EW2G6 P6625</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>ES 13FEB26 7200 C</t>
+          <t>ES 13FEB26 6625 P</t>
         </is>
       </c>
       <c r="H35" t="n">
         <v>50</v>
       </c>
       <c r="I35" t="n">
-        <v>7200</v>
+        <v>6625</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3184,42 +3355,47 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M35" t="n">
         <v>-2</v>
       </c>
       <c r="N35" t="n">
-        <v>5.3</v>
+        <v>20.75</v>
       </c>
       <c r="O35" t="n">
-        <v>-530</v>
+        <v>-2075</v>
       </c>
       <c r="P35" t="n">
-        <v>18.9716</v>
+        <v>42.2216</v>
       </c>
       <c r="Q35" t="n">
-        <v>18.9716</v>
+        <v>42.2216</v>
       </c>
       <c r="R35" t="n">
-        <v>-1897.16</v>
+        <v>-4222.16</v>
       </c>
       <c r="S35" t="n">
-        <v>1367.16</v>
+        <v>2147.16</v>
       </c>
       <c r="T35" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U35" t="n">
-        <v>-530</v>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>CME</t>
+        </is>
+      </c>
+      <c r="V35" t="n">
+        <v>-2075</v>
       </c>
     </row>
     <row r="36">
@@ -3238,57 +3414,78 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>CASH</t>
+          <t>FOP</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>EW2G6 C7200</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Cash Balance (Total USD)</t>
+          <t>ES 13FEB26 7200 C</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>1</v>
-      </c>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="inlineStr"/>
-      <c r="K36" t="inlineStr"/>
+        <v>50</v>
+      </c>
+      <c r="I36" t="n">
+        <v>7200</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>112212.482841557</v>
+        <v>-2</v>
       </c>
       <c r="N36" t="n">
-        <v>1</v>
+        <v>4.4</v>
       </c>
       <c r="O36" t="n">
-        <v>112212.482841557</v>
-      </c>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
+        <v>-440</v>
+      </c>
+      <c r="P36" t="n">
+        <v>18.9716</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>18.9716</v>
+      </c>
+      <c r="R36" t="n">
+        <v>-1897.16</v>
+      </c>
       <c r="S36" t="n">
-        <v>0</v>
+        <v>1457.16</v>
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>Long</t>
-        </is>
-      </c>
-      <c r="U36" t="n">
-        <v>112212.482841557</v>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>CME</t>
+        </is>
+      </c>
+      <c r="V36" t="n">
+        <v>-440</v>
       </c>
     </row>
   </sheetData>
@@ -3302,7 +3499,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3413,6 +3610,11 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
+          <t>ListingExchange</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
           <t>PositionValueUSD</t>
         </is>
       </c>
@@ -3429,7 +3631,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.1686</v>
+        <v>1.1828</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -3459,7 +3661,7 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -3488,8 +3690,13 @@
           <t>Long</t>
         </is>
       </c>
-      <c r="U2" t="n">
-        <v>53755.60000000001</v>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>IBIS</t>
+        </is>
+      </c>
+      <c r="V2" t="n">
+        <v>54408.8</v>
       </c>
     </row>
     <row r="3">
@@ -3504,7 +3711,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.1686</v>
+        <v>1.1828</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -3534,17 +3741,17 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M3" t="n">
         <v>5</v>
       </c>
       <c r="N3" t="n">
-        <v>585.2</v>
+        <v>591.4</v>
       </c>
       <c r="O3" t="n">
-        <v>2926</v>
+        <v>2957</v>
       </c>
       <c r="P3" t="n">
         <v>624.1</v>
@@ -3556,15 +3763,20 @@
         <v>3120.5</v>
       </c>
       <c r="S3" t="n">
-        <v>-194.5</v>
+        <v>-163.5</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U3" t="n">
-        <v>3419.3236</v>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>SBF</t>
+        </is>
+      </c>
+      <c r="V3" t="n">
+        <v>3497.5396</v>
       </c>
     </row>
     <row r="4">
@@ -3579,7 +3791,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.1686</v>
+        <v>1.1828</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -3609,17 +3821,17 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M4" t="n">
         <v>3</v>
       </c>
       <c r="N4" t="n">
-        <v>2098</v>
+        <v>2130</v>
       </c>
       <c r="O4" t="n">
-        <v>6294</v>
+        <v>6390</v>
       </c>
       <c r="P4" t="n">
         <v>2127.063</v>
@@ -3631,15 +3843,20 @@
         <v>6381.189</v>
       </c>
       <c r="S4" t="n">
-        <v>-87.18899999999999</v>
+        <v>8.811</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U4" t="n">
-        <v>7355.1684</v>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>SBF</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>7558.092000000001</v>
       </c>
     </row>
     <row r="5">
@@ -3654,7 +3871,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.1686</v>
+        <v>1.1828</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -3684,17 +3901,17 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M5" t="n">
         <v>400</v>
       </c>
       <c r="N5" t="n">
-        <v>147</v>
+        <v>147.72</v>
       </c>
       <c r="O5" t="n">
-        <v>58800</v>
+        <v>59088</v>
       </c>
       <c r="P5" t="n">
         <v>146.3403336</v>
@@ -3706,15 +3923,20 @@
         <v>58536.13344</v>
       </c>
       <c r="S5" t="n">
-        <v>263.86656</v>
+        <v>551.86656</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U5" t="n">
-        <v>68713.68000000001</v>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>IBIS2</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>69889.2864</v>
       </c>
     </row>
     <row r="6">
@@ -3729,7 +3951,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.77847</v>
+        <v>0.7861900000000001</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -3759,17 +3981,17 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M6" t="n">
         <v>10000</v>
       </c>
       <c r="N6" t="n">
-        <v>4.888</v>
+        <v>4.97</v>
       </c>
       <c r="O6" t="n">
-        <v>48880</v>
+        <v>49700</v>
       </c>
       <c r="P6" t="n">
         <v>3.81181816</v>
@@ -3781,15 +4003,20 @@
         <v>38118.1816</v>
       </c>
       <c r="S6" t="n">
-        <v>10761.8184</v>
+        <v>11581.8184</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U6" t="n">
-        <v>38051.6136</v>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>SGX</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>39073.643</v>
       </c>
     </row>
     <row r="7">
@@ -3804,7 +4031,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.77847</v>
+        <v>0.7861900000000001</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -3834,17 +4061,17 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M7" t="n">
         <v>10</v>
       </c>
       <c r="N7" t="n">
-        <v>574.1</v>
+        <v>577.5</v>
       </c>
       <c r="O7" t="n">
-        <v>5741</v>
+        <v>5775</v>
       </c>
       <c r="P7" t="n">
         <v>544.755456</v>
@@ -3856,15 +4083,20 @@
         <v>5447.55456</v>
       </c>
       <c r="S7" t="n">
-        <v>293.44544</v>
+        <v>327.44544</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U7" t="n">
-        <v>4469.19627</v>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>SGX</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>4540.24725</v>
       </c>
     </row>
     <row r="8">
@@ -3909,17 +4141,17 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M8" t="n">
         <v>200</v>
       </c>
       <c r="N8" t="n">
-        <v>12.49</v>
+        <v>12.4</v>
       </c>
       <c r="O8" t="n">
-        <v>2498</v>
+        <v>2480</v>
       </c>
       <c r="P8" t="n">
         <v>12.7</v>
@@ -3931,15 +4163,20 @@
         <v>2540</v>
       </c>
       <c r="S8" t="n">
-        <v>-42</v>
+        <v>-60</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U8" t="n">
-        <v>2498</v>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>ARCA</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>2480</v>
       </c>
     </row>
     <row r="9">
@@ -3984,17 +4221,17 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M9" t="n">
         <v>15</v>
       </c>
       <c r="N9" t="n">
-        <v>1448.2</v>
+        <v>1470.8</v>
       </c>
       <c r="O9" t="n">
-        <v>21723</v>
+        <v>22062</v>
       </c>
       <c r="P9" t="n">
         <v>1461.150733333</v>
@@ -4006,15 +4243,20 @@
         <v>21917.261</v>
       </c>
       <c r="S9" t="n">
-        <v>-194.261</v>
+        <v>144.739</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U9" t="n">
-        <v>21723</v>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>EBS</t>
+        </is>
+      </c>
+      <c r="V9" t="n">
+        <v>22062</v>
       </c>
     </row>
     <row r="10">
@@ -4059,17 +4301,17 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M10" t="n">
         <v>3000</v>
       </c>
       <c r="N10" t="n">
-        <v>5.481</v>
+        <v>5.526</v>
       </c>
       <c r="O10" t="n">
-        <v>16443</v>
+        <v>16578</v>
       </c>
       <c r="P10" t="n">
         <v>5.552814967</v>
@@ -4081,15 +4323,20 @@
         <v>16658.4449</v>
       </c>
       <c r="S10" t="n">
-        <v>-215.4449</v>
+        <v>-80.4449</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U10" t="n">
-        <v>16443</v>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>EBS</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>16578</v>
       </c>
     </row>
     <row r="11">
@@ -4113,17 +4360,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>HEAL</t>
+          <t>GOOGL</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ISHR HEALTHCARE INNOVATION</t>
+          <t>ALPHABET INC-CL A</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -4134,37 +4381,42 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="N11" t="n">
-        <v>9.43</v>
+        <v>327.93</v>
       </c>
       <c r="O11" t="n">
-        <v>9430</v>
+        <v>32793</v>
       </c>
       <c r="P11" t="n">
-        <v>9.405900600000001</v>
+        <v>331.87755</v>
       </c>
       <c r="Q11" t="n">
-        <v>9.405900600000001</v>
+        <v>331.87755</v>
       </c>
       <c r="R11" t="n">
-        <v>9405.900600000001</v>
+        <v>33187.755</v>
       </c>
       <c r="S11" t="n">
-        <v>24.0994</v>
+        <v>-394.755</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U11" t="n">
-        <v>9430</v>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v>32793</v>
       </c>
     </row>
     <row r="12">
@@ -4188,17 +4440,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>IBKR</t>
+          <t>HEAL</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>INTERACTIVE BROKERS GRO-CL A</t>
+          <t>ISHR HEALTHCARE INNOVATION</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -4209,37 +4461,42 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>16.8448</v>
+        <v>1000</v>
       </c>
       <c r="N12" t="n">
-        <v>75.8</v>
+        <v>9.494999999999999</v>
       </c>
       <c r="O12" t="n">
-        <v>1276.84</v>
+        <v>9495</v>
       </c>
       <c r="P12" t="n">
-        <v>20.721325216</v>
+        <v>9.405900600000001</v>
       </c>
       <c r="Q12" t="n">
-        <v>20.721325216</v>
+        <v>9.405900600000001</v>
       </c>
       <c r="R12" t="n">
-        <v>349.046579</v>
+        <v>9405.900600000001</v>
       </c>
       <c r="S12" t="n">
-        <v>927.793421</v>
+        <v>89.0994</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U12" t="n">
-        <v>1276.84</v>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>LSEETF</t>
+        </is>
+      </c>
+      <c r="V12" t="n">
+        <v>9495</v>
       </c>
     </row>
     <row r="13">
@@ -4263,17 +4520,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>INRA</t>
+          <t>IBKR</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>ISHAR GL CL EN TR UCI ETF-US</t>
+          <t>INTERACTIVE BROKERS GRO-CL A</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -4284,37 +4541,42 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>385</v>
+        <v>16.8448</v>
       </c>
       <c r="N13" t="n">
-        <v>26.0432</v>
+        <v>77.58</v>
       </c>
       <c r="O13" t="n">
-        <v>10026.63</v>
+        <v>1306.82</v>
       </c>
       <c r="P13" t="n">
-        <v>25.997158151</v>
+        <v>20.721325216</v>
       </c>
       <c r="Q13" t="n">
-        <v>25.997158151</v>
+        <v>20.721325216</v>
       </c>
       <c r="R13" t="n">
-        <v>10008.905888</v>
+        <v>349.046579</v>
       </c>
       <c r="S13" t="n">
-        <v>17.724112</v>
+        <v>957.773421</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U13" t="n">
-        <v>10026.63</v>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>NASDAQ</t>
+        </is>
+      </c>
+      <c r="V13" t="n">
+        <v>1306.82</v>
       </c>
     </row>
     <row r="14">
@@ -4338,17 +4600,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>INRA</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>JPMORGAN CHASE &amp; CO</t>
+          <t>ISHAR GL CL EN TR UCI ETF-US</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -4359,37 +4621,42 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>100</v>
+        <v>385</v>
       </c>
       <c r="N14" t="n">
-        <v>302.04</v>
+        <v>27.0092</v>
       </c>
       <c r="O14" t="n">
-        <v>30204</v>
+        <v>10398.54</v>
       </c>
       <c r="P14" t="n">
-        <v>314.1727</v>
+        <v>25.997158151</v>
       </c>
       <c r="Q14" t="n">
-        <v>314.1727</v>
+        <v>25.997158151</v>
       </c>
       <c r="R14" t="n">
-        <v>31417.27</v>
+        <v>10008.905888</v>
       </c>
       <c r="S14" t="n">
-        <v>-1213.27</v>
+        <v>389.634112</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U14" t="n">
-        <v>30204</v>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>AEB</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>10398.54</v>
       </c>
     </row>
     <row r="15">
@@ -4413,17 +4680,17 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>LOCK</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ISHARES DIGITAL SCRTY USD-A</t>
+          <t>JPMORGAN CHASE &amp; CO</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -4434,37 +4701,42 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="N15" t="n">
-        <v>9.952</v>
+        <v>297.72</v>
       </c>
       <c r="O15" t="n">
-        <v>9952</v>
+        <v>29772</v>
       </c>
       <c r="P15" t="n">
-        <v>10.229112</v>
+        <v>298.02</v>
       </c>
       <c r="Q15" t="n">
-        <v>10.229112</v>
+        <v>298.02</v>
       </c>
       <c r="R15" t="n">
-        <v>10229.112</v>
+        <v>29802</v>
       </c>
       <c r="S15" t="n">
-        <v>-277.112</v>
+        <v>-30</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U15" t="n">
-        <v>9952</v>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>29772</v>
       </c>
     </row>
     <row r="16">
@@ -4493,12 +4765,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>VWRA</t>
+          <t>LOCK</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>VANG FTSE AW USDA</t>
+          <t>ISHARES DIGITAL SCRTY USD-A</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -4509,37 +4781,42 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="N16" t="n">
-        <v>172.18</v>
+        <v>10.02</v>
       </c>
       <c r="O16" t="n">
-        <v>137744</v>
+        <v>10020</v>
       </c>
       <c r="P16" t="n">
-        <v>170.683661681</v>
+        <v>10.229112</v>
       </c>
       <c r="Q16" t="n">
-        <v>170.683661681</v>
+        <v>10.229112</v>
       </c>
       <c r="R16" t="n">
-        <v>136546.929345</v>
+        <v>10229.112</v>
       </c>
       <c r="S16" t="n">
-        <v>1197.070655</v>
+        <v>-209.112</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U16" t="n">
-        <v>137744</v>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>LSEETF</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
+        <v>10020</v>
       </c>
     </row>
     <row r="17">
@@ -4558,73 +4835,68 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>OPT</t>
+          <t>STK</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>QQQ   260220P00605000</t>
+          <t>VWRA</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>QQQ 20FEB26 605 P</t>
+          <t>VANG FTSE AW USDA</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>100</v>
-      </c>
-      <c r="I17" t="n">
-        <v>605</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>2026-02-20</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>1</v>
+        <v>800</v>
       </c>
       <c r="N17" t="n">
-        <v>8.945</v>
+        <v>173.74</v>
       </c>
       <c r="O17" t="n">
-        <v>894.5</v>
+        <v>138992</v>
       </c>
       <c r="P17" t="n">
-        <v>10.9285875</v>
+        <v>170.683661681</v>
       </c>
       <c r="Q17" t="n">
-        <v>10.9285875</v>
+        <v>170.683661681</v>
       </c>
       <c r="R17" t="n">
-        <v>1092.85875</v>
+        <v>136546.929345</v>
       </c>
       <c r="S17" t="n">
-        <v>-198.35875</v>
+        <v>2445.070655</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
           <t>Long</t>
         </is>
       </c>
-      <c r="U17" t="n">
-        <v>894.5</v>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>LSEETF</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
+        <v>138992</v>
       </c>
     </row>
     <row r="18">
@@ -4653,23 +4925,23 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>GOOGL 260130P00310000</t>
+          <t>QQQ   260220P00605000</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>GOOGL 30JAN26 310 P</t>
+          <t>QQQ 20FEB26 605 P</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>100</v>
       </c>
       <c r="I18" t="n">
-        <v>310</v>
+        <v>605</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -4679,37 +4951,42 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="N18" t="n">
-        <v>1.16</v>
+        <v>6.34</v>
       </c>
       <c r="O18" t="n">
-        <v>-116</v>
+        <v>634</v>
       </c>
       <c r="P18" t="n">
-        <v>7.2294796</v>
+        <v>10.9285875</v>
       </c>
       <c r="Q18" t="n">
-        <v>7.2294796</v>
+        <v>10.9285875</v>
       </c>
       <c r="R18" t="n">
-        <v>-722.94796</v>
+        <v>1092.85875</v>
       </c>
       <c r="S18" t="n">
-        <v>606.94796</v>
+        <v>-458.85875</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>Short</t>
-        </is>
-      </c>
-      <c r="U18" t="n">
-        <v>-116</v>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V18" t="n">
+        <v>634</v>
       </c>
     </row>
     <row r="19">
@@ -4733,68 +5010,73 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>GOOGL 260220P00315000</t>
+          <t>GOOGL 260206C00335000</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>GOOGL 20FEB26 315 P</t>
+          <t>GOOGL 06FEB26 335 C</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>100</v>
       </c>
       <c r="I19" t="n">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M19" t="n">
         <v>-1</v>
       </c>
       <c r="N19" t="n">
-        <v>7.925</v>
+        <v>8.275</v>
       </c>
       <c r="O19" t="n">
-        <v>-792.5</v>
+        <v>-827.5</v>
       </c>
       <c r="P19" t="n">
-        <v>8.729479599999999</v>
+        <v>10.0494796</v>
       </c>
       <c r="Q19" t="n">
-        <v>8.729479599999999</v>
+        <v>10.0494796</v>
       </c>
       <c r="R19" t="n">
-        <v>-872.94796</v>
+        <v>-1004.94796</v>
       </c>
       <c r="S19" t="n">
-        <v>80.44795999999999</v>
+        <v>177.44796</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U19" t="n">
-        <v>-792.5</v>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V19" t="n">
+        <v>-827.5</v>
       </c>
     </row>
     <row r="20">
@@ -4818,68 +5100,73 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>JPM   260130C00325000</t>
+          <t>GOOGL 260220P00315000</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>JPM 30JAN26 325 C</t>
+          <t>GOOGL 20FEB26 315 P</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>100</v>
       </c>
       <c r="I20" t="n">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M20" t="n">
         <v>-1</v>
       </c>
       <c r="N20" t="n">
-        <v>0.1325</v>
+        <v>7.675</v>
       </c>
       <c r="O20" t="n">
-        <v>-13.25</v>
+        <v>-767.5</v>
       </c>
       <c r="P20" t="n">
-        <v>2.3994796</v>
+        <v>8.729479599999999</v>
       </c>
       <c r="Q20" t="n">
-        <v>2.3994796</v>
+        <v>8.729479599999999</v>
       </c>
       <c r="R20" t="n">
-        <v>-239.94796</v>
+        <v>-872.94796</v>
       </c>
       <c r="S20" t="n">
-        <v>226.69796</v>
+        <v>105.44796</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U20" t="n">
-        <v>-13.25</v>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V20" t="n">
+        <v>-767.5</v>
       </c>
     </row>
     <row r="21">
@@ -4908,23 +5195,23 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>QQQ   260130P00608000</t>
+          <t>JPM   260206P00287500</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>QQQ 30JAN26 608 P</t>
+          <t>JPM 06FEB26 287.5 P</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>100</v>
       </c>
       <c r="I21" t="n">
-        <v>608</v>
+        <v>287.5</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -4934,37 +5221,42 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M21" t="n">
         <v>-1</v>
       </c>
       <c r="N21" t="n">
-        <v>4.79</v>
+        <v>1.695</v>
       </c>
       <c r="O21" t="n">
-        <v>-479</v>
+        <v>-169.5</v>
       </c>
       <c r="P21" t="n">
-        <v>6.0594796</v>
+        <v>1.7094796</v>
       </c>
       <c r="Q21" t="n">
-        <v>6.0594796</v>
+        <v>1.7094796</v>
       </c>
       <c r="R21" t="n">
-        <v>-605.94796</v>
+        <v>-170.94796</v>
       </c>
       <c r="S21" t="n">
-        <v>126.94796</v>
+        <v>1.44796</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U21" t="n">
-        <v>-479</v>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V21" t="n">
+        <v>-169.5</v>
       </c>
     </row>
     <row r="22">
@@ -4988,68 +5280,73 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>QQQ   260220P00570000</t>
+          <t>JPM   260206C00315000</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>QQQ 20FEB26 570 P</t>
+          <t>JPM 06FEB26 315 C</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>100</v>
       </c>
       <c r="I22" t="n">
-        <v>570</v>
+        <v>315</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="M22" t="n">
         <v>-1</v>
       </c>
       <c r="N22" t="n">
-        <v>2.995</v>
+        <v>0.585</v>
       </c>
       <c r="O22" t="n">
-        <v>-299.5</v>
+        <v>-58.5</v>
       </c>
       <c r="P22" t="n">
-        <v>3.8261796</v>
+        <v>2.0294546</v>
       </c>
       <c r="Q22" t="n">
-        <v>3.8261796</v>
+        <v>2.0294546</v>
       </c>
       <c r="R22" t="n">
-        <v>-382.61796</v>
+        <v>-202.94546</v>
       </c>
       <c r="S22" t="n">
-        <v>83.11796</v>
+        <v>144.44546</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
           <t>Short</t>
         </is>
       </c>
-      <c r="U22" t="n">
-        <v>-299.5</v>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V22" t="n">
+        <v>-58.5</v>
       </c>
     </row>
     <row r="23">
@@ -5068,57 +5365,168 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>CASH</t>
+          <t>OPT</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>QQQ   260130P00608000</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>QQQ 30JAN26 608 P</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>100</v>
+      </c>
+      <c r="I23" t="n">
+        <v>608</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N23" t="n">
+        <v>2.105</v>
+      </c>
+      <c r="O23" t="n">
+        <v>-210.5</v>
+      </c>
+      <c r="P23" t="n">
+        <v>6.0594796</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>6.0594796</v>
+      </c>
+      <c r="R23" t="n">
+        <v>-605.94796</v>
+      </c>
+      <c r="S23" t="n">
+        <v>395.44796</v>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V23" t="n">
+        <v>-210.5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>U6565621</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Cash Balance (Total USD)</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>1</v>
-      </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>2026-01-21</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>136534.613674778</v>
-      </c>
-      <c r="N23" t="n">
-        <v>1</v>
-      </c>
-      <c r="O23" t="n">
-        <v>136534.613674778</v>
-      </c>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>Long</t>
-        </is>
-      </c>
-      <c r="U23" t="n">
-        <v>136534.613674778</v>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>OPT</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>QQQ   260220P00570000</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>QQQ 20FEB26 570 P</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>100</v>
+      </c>
+      <c r="I24" t="n">
+        <v>570</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>2026-02-20</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>2026-01-23</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1.895</v>
+      </c>
+      <c r="O24" t="n">
+        <v>-189.5</v>
+      </c>
+      <c r="P24" t="n">
+        <v>3.8261796</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>3.8261796</v>
+      </c>
+      <c r="R24" t="n">
+        <v>-382.61796</v>
+      </c>
+      <c r="S24" t="n">
+        <v>193.11796</v>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>CBOE</t>
+        </is>
+      </c>
+      <c r="V24" t="n">
+        <v>-189.5</v>
       </c>
     </row>
   </sheetData>
@@ -5127,6 +5535,119 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Account</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Positions Value</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Cash Balance</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Account Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HK</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>$344,962.48</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>$103,358.02</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$448,320.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AL</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>$451,275.97</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$105,735.07</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$557,011.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>$796,238.45</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$209,093.09</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$1,005,331.54</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5170,14 +5691,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-23 11:52:55</t>
+          <t>2026-01-25 19:12:00</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>35</v>
       </c>
       <c r="C2" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update IBKR positions - 2026-01-31
</commit_message>
<xml_diff>
--- a/projects/fetch-ibkr-positions.xlsx
+++ b/projects/fetch-ibkr-positions.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.3084</v>
+        <v>1.2935</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -590,29 +590,29 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="N2" t="n">
-        <v>410.05</v>
+        <v>411.6</v>
       </c>
       <c r="O2" t="n">
-        <v>16402</v>
+        <v>20580</v>
       </c>
       <c r="P2" t="n">
-        <v>419.45012025</v>
+        <v>418.0600962</v>
       </c>
       <c r="Q2" t="n">
-        <v>419.45012025</v>
+        <v>418.0600962</v>
       </c>
       <c r="R2" t="n">
-        <v>16778.00481</v>
+        <v>20903.00481</v>
       </c>
       <c r="S2" t="n">
-        <v>-376.00481</v>
+        <v>-323.00481</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
         </is>
       </c>
       <c r="V2" t="n">
-        <v>21460.3768</v>
+        <v>26620.23</v>
       </c>
     </row>
     <row r="3">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.3084</v>
+        <v>1.2935</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -670,17 +670,17 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M3" t="n">
         <v>4500</v>
       </c>
       <c r="N3" t="n">
-        <v>3.5335</v>
+        <v>3.5425</v>
       </c>
       <c r="O3" t="n">
-        <v>15900.75</v>
+        <v>15941.25</v>
       </c>
       <c r="P3" t="n">
         <v>3.58108965</v>
@@ -692,7 +692,7 @@
         <v>16114.903425</v>
       </c>
       <c r="S3" t="n">
-        <v>-214.153425</v>
+        <v>-173.653425</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="V3" t="n">
-        <v>20804.5413</v>
+        <v>20620.006875</v>
       </c>
     </row>
     <row r="4">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.3084</v>
+        <v>1.2935</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -750,17 +750,17 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M4" t="n">
         <v>150</v>
       </c>
       <c r="N4" t="n">
-        <v>63.64</v>
+        <v>63.41</v>
       </c>
       <c r="O4" t="n">
-        <v>9546</v>
+        <v>9511.5</v>
       </c>
       <c r="P4" t="n">
         <v>64.678533333</v>
@@ -772,7 +772,7 @@
         <v>9701.780000000001</v>
       </c>
       <c r="S4" t="n">
-        <v>-155.78</v>
+        <v>-190.28</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="V4" t="n">
-        <v>12489.9864</v>
+        <v>12303.12525</v>
       </c>
     </row>
     <row r="5">
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.14399</v>
+        <v>0.1437</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -830,17 +830,17 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M5" t="n">
         <v>2000</v>
       </c>
       <c r="N5" t="n">
-        <v>31.92</v>
+        <v>31.58</v>
       </c>
       <c r="O5" t="n">
-        <v>63840</v>
+        <v>63160</v>
       </c>
       <c r="P5" t="n">
         <v>31.16579949</v>
@@ -852,7 +852,7 @@
         <v>62331.59898</v>
       </c>
       <c r="S5" t="n">
-        <v>1508.40102</v>
+        <v>828.40102</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="V5" t="n">
-        <v>9192.321600000001</v>
+        <v>9076.092000000001</v>
       </c>
     </row>
     <row r="6">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.1971</v>
+        <v>1.185</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -910,17 +910,17 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M6" t="n">
         <v>4000</v>
       </c>
       <c r="N6" t="n">
-        <v>4.5805</v>
+        <v>4.5705</v>
       </c>
       <c r="O6" t="n">
-        <v>18322</v>
+        <v>18282</v>
       </c>
       <c r="P6" t="n">
         <v>4.66216992</v>
@@ -932,7 +932,7 @@
         <v>18648.67968</v>
       </c>
       <c r="S6" t="n">
-        <v>-326.67968</v>
+        <v>-366.67968</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="V6" t="n">
-        <v>21933.2662</v>
+        <v>21664.17</v>
       </c>
     </row>
     <row r="7">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.79082</v>
+        <v>0.78593</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -990,17 +990,17 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M7" t="n">
         <v>5000</v>
       </c>
       <c r="N7" t="n">
-        <v>5.019</v>
+        <v>4.996</v>
       </c>
       <c r="O7" t="n">
-        <v>25095</v>
+        <v>24980</v>
       </c>
       <c r="P7" t="n">
         <v>4.54124249</v>
@@ -1012,7 +1012,7 @@
         <v>22706.21245</v>
       </c>
       <c r="S7" t="n">
-        <v>2388.78755</v>
+        <v>2273.78755</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="V7" t="n">
-        <v>19845.6279</v>
+        <v>19632.5314</v>
       </c>
     </row>
     <row r="8">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.79082</v>
+        <v>0.78593</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1070,29 +1070,29 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="N8" t="n">
-        <v>640.2</v>
+        <v>595</v>
       </c>
       <c r="O8" t="n">
-        <v>32010</v>
+        <v>14875</v>
       </c>
       <c r="P8" t="n">
-        <v>432.4596912</v>
+        <v>430.033752</v>
       </c>
       <c r="Q8" t="n">
-        <v>432.4596912</v>
+        <v>430.033752</v>
       </c>
       <c r="R8" t="n">
-        <v>21622.98456</v>
+        <v>10750.8438</v>
       </c>
       <c r="S8" t="n">
-        <v>10387.01544</v>
+        <v>4124.1562</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="V8" t="n">
-        <v>25314.1482</v>
+        <v>11690.70875</v>
       </c>
     </row>
     <row r="9">
@@ -1150,17 +1150,17 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M9" t="n">
         <v>100</v>
       </c>
       <c r="N9" t="n">
-        <v>11.66</v>
+        <v>11.6</v>
       </c>
       <c r="O9" t="n">
-        <v>1166</v>
+        <v>1160</v>
       </c>
       <c r="P9" t="n">
         <v>12.97</v>
@@ -1172,7 +1172,7 @@
         <v>1297</v>
       </c>
       <c r="S9" t="n">
-        <v>-131</v>
+        <v>-137</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -1185,7 +1185,7 @@
         </is>
       </c>
       <c r="V9" t="n">
-        <v>1166</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="10">
@@ -1230,17 +1230,17 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M10" t="n">
         <v>50</v>
       </c>
       <c r="N10" t="n">
-        <v>53.37</v>
+        <v>52.48</v>
       </c>
       <c r="O10" t="n">
-        <v>2668.5</v>
+        <v>2624</v>
       </c>
       <c r="P10" t="n">
         <v>46.285022</v>
@@ -1252,7 +1252,7 @@
         <v>2314.2511</v>
       </c>
       <c r="S10" t="n">
-        <v>354.2489</v>
+        <v>309.7489</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="V10" t="n">
-        <v>2668.5</v>
+        <v>2624</v>
       </c>
     </row>
     <row r="11">
@@ -1310,17 +1310,17 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M11" t="n">
         <v>100</v>
       </c>
       <c r="N11" t="n">
-        <v>12.06</v>
+        <v>11.72</v>
       </c>
       <c r="O11" t="n">
-        <v>1206</v>
+        <v>1172</v>
       </c>
       <c r="P11" t="n">
         <v>12.49</v>
@@ -1332,7 +1332,7 @@
         <v>1249</v>
       </c>
       <c r="S11" t="n">
-        <v>-43</v>
+        <v>-77</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -1345,7 +1345,7 @@
         </is>
       </c>
       <c r="V11" t="n">
-        <v>1206</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="12">
@@ -1390,17 +1390,17 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M12" t="n">
         <v>15</v>
       </c>
       <c r="N12" t="n">
-        <v>1466.4</v>
+        <v>1474.8</v>
       </c>
       <c r="O12" t="n">
-        <v>21996</v>
+        <v>22122</v>
       </c>
       <c r="P12" t="n">
         <v>1474.989023133</v>
@@ -1412,7 +1412,7 @@
         <v>22124.835347</v>
       </c>
       <c r="S12" t="n">
-        <v>-128.835347</v>
+        <v>-2.835347</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
@@ -1425,7 +1425,7 @@
         </is>
       </c>
       <c r="V12" t="n">
-        <v>21996</v>
+        <v>22122</v>
       </c>
     </row>
     <row r="13">
@@ -1470,17 +1470,17 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M13" t="n">
         <v>100</v>
       </c>
       <c r="N13" t="n">
-        <v>338.25</v>
+        <v>338</v>
       </c>
       <c r="O13" t="n">
-        <v>33825</v>
+        <v>33800</v>
       </c>
       <c r="P13" t="n">
         <v>312.15</v>
@@ -1492,7 +1492,7 @@
         <v>31215</v>
       </c>
       <c r="S13" t="n">
-        <v>2610</v>
+        <v>2585</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -1505,7 +1505,7 @@
         </is>
       </c>
       <c r="V13" t="n">
-        <v>33825</v>
+        <v>33800</v>
       </c>
     </row>
     <row r="14">
@@ -1550,17 +1550,17 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M14" t="n">
         <v>1000</v>
       </c>
       <c r="N14" t="n">
-        <v>9.3725</v>
+        <v>9.2925</v>
       </c>
       <c r="O14" t="n">
-        <v>9372.5</v>
+        <v>9292.5</v>
       </c>
       <c r="P14" t="n">
         <v>9.424709999999999</v>
@@ -1572,7 +1572,7 @@
         <v>9424.709999999999</v>
       </c>
       <c r="S14" t="n">
-        <v>-52.21</v>
+        <v>-132.21</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
@@ -1585,7 +1585,7 @@
         </is>
       </c>
       <c r="V14" t="n">
-        <v>9372.5</v>
+        <v>9292.5</v>
       </c>
     </row>
     <row r="15">
@@ -1630,17 +1630,17 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M15" t="n">
         <v>385</v>
       </c>
       <c r="N15" t="n">
-        <v>27.0739</v>
+        <v>27.0617</v>
       </c>
       <c r="O15" t="n">
-        <v>10423.45</v>
+        <v>10418.75</v>
       </c>
       <c r="P15" t="n">
         <v>26.012734603</v>
@@ -1652,7 +1652,7 @@
         <v>10014.902822</v>
       </c>
       <c r="S15" t="n">
-        <v>408.547178</v>
+        <v>403.847178</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -1665,7 +1665,7 @@
         </is>
       </c>
       <c r="V15" t="n">
-        <v>10423.45</v>
+        <v>10418.75</v>
       </c>
     </row>
     <row r="16">
@@ -1710,29 +1710,29 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N16" t="n">
-        <v>32.61</v>
+        <v>33.37</v>
       </c>
       <c r="O16" t="n">
-        <v>1630.5</v>
+        <v>3337</v>
       </c>
       <c r="P16" t="n">
-        <v>36.96000022</v>
+        <v>35.26000011</v>
       </c>
       <c r="Q16" t="n">
-        <v>36.96000022</v>
+        <v>35.26000011</v>
       </c>
       <c r="R16" t="n">
-        <v>1848.000011</v>
+        <v>3526.000011</v>
       </c>
       <c r="S16" t="n">
-        <v>-217.500011</v>
+        <v>-189.000011</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="V16" t="n">
-        <v>1630.5</v>
+        <v>3337</v>
       </c>
     </row>
     <row r="17">
@@ -1790,17 +1790,17 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M17" t="n">
         <v>1000</v>
       </c>
       <c r="N17" t="n">
-        <v>9.85</v>
+        <v>9.824</v>
       </c>
       <c r="O17" t="n">
-        <v>9850</v>
+        <v>9824</v>
       </c>
       <c r="P17" t="n">
         <v>10.2267108</v>
@@ -1812,7 +1812,7 @@
         <v>10226.7108</v>
       </c>
       <c r="S17" t="n">
-        <v>-376.7108</v>
+        <v>-402.7108</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="V17" t="n">
-        <v>9850</v>
+        <v>9824</v>
       </c>
     </row>
     <row r="18">
@@ -1870,17 +1870,17 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M18" t="n">
         <v>200</v>
       </c>
       <c r="N18" t="n">
-        <v>192.51</v>
+        <v>191.13</v>
       </c>
       <c r="O18" t="n">
-        <v>38502</v>
+        <v>38226</v>
       </c>
       <c r="P18" t="n">
         <v>185.216422</v>
@@ -1892,7 +1892,7 @@
         <v>37043.2844</v>
       </c>
       <c r="S18" t="n">
-        <v>1458.7156</v>
+        <v>1182.7156</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
@@ -1905,7 +1905,7 @@
         </is>
       </c>
       <c r="V18" t="n">
-        <v>38502</v>
+        <v>38226</v>
       </c>
     </row>
     <row r="19">
@@ -1950,17 +1950,17 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M19" t="n">
         <v>100</v>
       </c>
       <c r="N19" t="n">
-        <v>169.01</v>
+        <v>164.58</v>
       </c>
       <c r="O19" t="n">
-        <v>16901</v>
+        <v>16458</v>
       </c>
       <c r="P19" t="n">
         <v>205.3357044</v>
@@ -1972,7 +1972,7 @@
         <v>20533.57044</v>
       </c>
       <c r="S19" t="n">
-        <v>-3632.57044</v>
+        <v>-4075.57044</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
@@ -1985,7 +1985,7 @@
         </is>
       </c>
       <c r="V19" t="n">
-        <v>16901</v>
+        <v>16458</v>
       </c>
     </row>
     <row r="20">
@@ -2030,29 +2030,29 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N20" t="n">
-        <v>121.9</v>
+        <v>116.49</v>
       </c>
       <c r="O20" t="n">
-        <v>1219</v>
+        <v>2329.8</v>
       </c>
       <c r="P20" t="n">
-        <v>128.6</v>
+        <v>124.315</v>
       </c>
       <c r="Q20" t="n">
-        <v>128.6</v>
+        <v>124.315</v>
       </c>
       <c r="R20" t="n">
-        <v>1286</v>
+        <v>2486.3</v>
       </c>
       <c r="S20" t="n">
-        <v>-67</v>
+        <v>-156.5</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="V20" t="n">
-        <v>1219</v>
+        <v>2329.8</v>
       </c>
     </row>
     <row r="21">
@@ -2110,17 +2110,17 @@
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M21" t="n">
         <v>200</v>
       </c>
       <c r="N21" t="n">
-        <v>174.54</v>
+        <v>174.7</v>
       </c>
       <c r="O21" t="n">
-        <v>34908</v>
+        <v>34940</v>
       </c>
       <c r="P21" t="n">
         <v>171.74192805</v>
@@ -2132,7 +2132,7 @@
         <v>34348.38561</v>
       </c>
       <c r="S21" t="n">
-        <v>559.61439</v>
+        <v>591.61439</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="V21" t="n">
-        <v>34908</v>
+        <v>34940</v>
       </c>
     </row>
     <row r="22">
@@ -2200,17 +2200,17 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M22" t="n">
         <v>2</v>
       </c>
       <c r="N22" t="n">
-        <v>24.0436</v>
+        <v>25.8147</v>
       </c>
       <c r="O22" t="n">
-        <v>4808.72</v>
+        <v>5162.94</v>
       </c>
       <c r="P22" t="n">
         <v>23.4605</v>
@@ -2222,7 +2222,7 @@
         <v>4692.1</v>
       </c>
       <c r="S22" t="n">
-        <v>116.62</v>
+        <v>470.84</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
@@ -2235,7 +2235,7 @@
         </is>
       </c>
       <c r="V22" t="n">
-        <v>4808.72</v>
+        <v>5162.94</v>
       </c>
     </row>
     <row r="23">
@@ -2290,17 +2290,17 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M23" t="n">
         <v>2</v>
       </c>
       <c r="N23" t="n">
-        <v>20.615</v>
+        <v>21.1757</v>
       </c>
       <c r="O23" t="n">
-        <v>4123</v>
+        <v>4235.14</v>
       </c>
       <c r="P23" t="n">
         <v>20.1374875</v>
@@ -2312,7 +2312,7 @@
         <v>4027.4975</v>
       </c>
       <c r="S23" t="n">
-        <v>95.5025</v>
+        <v>207.6425</v>
       </c>
       <c r="T23" t="inlineStr">
         <is>
@@ -2325,7 +2325,7 @@
         </is>
       </c>
       <c r="V23" t="n">
-        <v>4123</v>
+        <v>4235.14</v>
       </c>
     </row>
     <row r="24">
@@ -2380,17 +2380,17 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M24" t="n">
         <v>2</v>
       </c>
       <c r="N24" t="n">
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="O24" t="n">
-        <v>800</v>
+        <v>875</v>
       </c>
       <c r="P24" t="n">
         <v>31.5284</v>
@@ -2402,7 +2402,7 @@
         <v>3152.84</v>
       </c>
       <c r="S24" t="n">
-        <v>-2352.84</v>
+        <v>-2277.84</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
@@ -2415,7 +2415,7 @@
         </is>
       </c>
       <c r="V24" t="n">
-        <v>800</v>
+        <v>875</v>
       </c>
     </row>
     <row r="25">
@@ -2470,17 +2470,17 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M25" t="n">
         <v>2</v>
       </c>
       <c r="N25" t="n">
-        <v>0.7</v>
+        <v>0.25</v>
       </c>
       <c r="O25" t="n">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="P25" t="n">
         <v>8.0284</v>
@@ -2492,7 +2492,7 @@
         <v>802.84</v>
       </c>
       <c r="S25" t="n">
-        <v>-732.84</v>
+        <v>-777.84</v>
       </c>
       <c r="T25" t="inlineStr">
         <is>
@@ -2505,7 +2505,7 @@
         </is>
       </c>
       <c r="V25" t="n">
-        <v>70</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
@@ -2560,17 +2560,17 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M26" t="n">
         <v>-1</v>
       </c>
       <c r="N26" t="n">
-        <v>4.5</v>
+        <v>4.2001</v>
       </c>
       <c r="O26" t="n">
-        <v>-450</v>
+        <v>-420.01</v>
       </c>
       <c r="P26" t="n">
         <v>7.2294546</v>
@@ -2582,7 +2582,7 @@
         <v>-722.94546</v>
       </c>
       <c r="S26" t="n">
-        <v>272.94546</v>
+        <v>302.93546</v>
       </c>
       <c r="T26" t="inlineStr">
         <is>
@@ -2595,7 +2595,7 @@
         </is>
       </c>
       <c r="V26" t="n">
-        <v>-450</v>
+        <v>-420.01</v>
       </c>
     </row>
     <row r="27">
@@ -2650,17 +2650,17 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M27" t="n">
         <v>-1</v>
       </c>
       <c r="N27" t="n">
-        <v>4.575</v>
+        <v>4.2262</v>
       </c>
       <c r="O27" t="n">
-        <v>-457.5</v>
+        <v>-422.62</v>
       </c>
       <c r="P27" t="n">
         <v>5.6494546</v>
@@ -2672,7 +2672,7 @@
         <v>-564.94546</v>
       </c>
       <c r="S27" t="n">
-        <v>107.44546</v>
+        <v>142.32546</v>
       </c>
       <c r="T27" t="inlineStr">
         <is>
@@ -2685,7 +2685,7 @@
         </is>
       </c>
       <c r="V27" t="n">
-        <v>-457.5</v>
+        <v>-422.62</v>
       </c>
     </row>
     <row r="28">
@@ -2714,55 +2714,55 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>NVDA  260130C00195000</t>
+          <t>ORCL  260213C00175000</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>NVDA 30JAN26 195 C</t>
+          <t>ORCL 13FEB26 175 C</t>
         </is>
       </c>
       <c r="H28" t="n">
         <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
           <t>2026-01-30</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>2026-01-29</t>
-        </is>
-      </c>
       <c r="M28" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="N28" t="n">
-        <v>0.5608</v>
+        <v>3.3</v>
       </c>
       <c r="O28" t="n">
-        <v>-112.16</v>
+        <v>-330</v>
       </c>
       <c r="P28" t="n">
-        <v>2.1886796</v>
+        <v>3.3094546</v>
       </c>
       <c r="Q28" t="n">
-        <v>2.1886796</v>
+        <v>3.3094546</v>
       </c>
       <c r="R28" t="n">
-        <v>-437.73592</v>
+        <v>-330.94546</v>
       </c>
       <c r="S28" t="n">
-        <v>325.57592</v>
+        <v>0.94546</v>
       </c>
       <c r="T28" t="inlineStr">
         <is>
@@ -2775,7 +2775,7 @@
         </is>
       </c>
       <c r="V28" t="n">
-        <v>-112.16</v>
+        <v>-330</v>
       </c>
     </row>
     <row r="29">
@@ -2804,23 +2804,23 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>ORCL  260213C00175000</t>
+          <t>ORCL  260220C00200000</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>ORCL 13FEB26 175 C</t>
+          <t>ORCL 20FEB26 200 C</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>100</v>
       </c>
       <c r="I29" t="n">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2830,29 +2830,29 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M29" t="n">
         <v>-1</v>
       </c>
       <c r="N29" t="n">
-        <v>5.5</v>
+        <v>0.745</v>
       </c>
       <c r="O29" t="n">
-        <v>-550</v>
+        <v>-74.5</v>
       </c>
       <c r="P29" t="n">
-        <v>3.3094546</v>
+        <v>2.3894796</v>
       </c>
       <c r="Q29" t="n">
-        <v>3.3094546</v>
+        <v>2.3894796</v>
       </c>
       <c r="R29" t="n">
-        <v>-330.94546</v>
+        <v>-238.94796</v>
       </c>
       <c r="S29" t="n">
-        <v>-219.05454</v>
+        <v>164.44796</v>
       </c>
       <c r="T29" t="inlineStr">
         <is>
@@ -2865,7 +2865,7 @@
         </is>
       </c>
       <c r="V29" t="n">
-        <v>-550</v>
+        <v>-74.5</v>
       </c>
     </row>
     <row r="30">
@@ -2889,60 +2889,60 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>ORCL  260220C00200000</t>
+          <t>QQQ   261218P00425000</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>ORCL 20FEB26 200 C</t>
+          <t>QQQ 18DEC26 425 P</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>100</v>
       </c>
       <c r="I30" t="n">
-        <v>200</v>
+        <v>425</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-12-18</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N30" t="n">
-        <v>1.335</v>
+        <v>7.1668</v>
       </c>
       <c r="O30" t="n">
-        <v>-133.5</v>
+        <v>-1433.36</v>
       </c>
       <c r="P30" t="n">
-        <v>2.3894796</v>
+        <v>6.3644671</v>
       </c>
       <c r="Q30" t="n">
-        <v>2.3894796</v>
+        <v>6.3644671</v>
       </c>
       <c r="R30" t="n">
-        <v>-238.94796</v>
+        <v>-1272.89342</v>
       </c>
       <c r="S30" t="n">
-        <v>105.44796</v>
+        <v>-160.46658</v>
       </c>
       <c r="T30" t="inlineStr">
         <is>
@@ -2955,7 +2955,7 @@
         </is>
       </c>
       <c r="V30" t="n">
-        <v>-133.5</v>
+        <v>-1433.36</v>
       </c>
     </row>
     <row r="31">
@@ -2984,19 +2984,19 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>QQQ   261218P00425000</t>
+          <t>SPY   261218P00505000</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>QQQ 18DEC26 425 P</t>
+          <t>SPY 18DEC26 505 P</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>425</v>
+        <v>505</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -3010,29 +3010,29 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M31" t="n">
         <v>-2</v>
       </c>
       <c r="N31" t="n">
-        <v>6.6444</v>
+        <v>7.865</v>
       </c>
       <c r="O31" t="n">
-        <v>-1328.88</v>
+        <v>-1573</v>
       </c>
       <c r="P31" t="n">
-        <v>6.3644671</v>
+        <v>7.3548796</v>
       </c>
       <c r="Q31" t="n">
-        <v>6.3644671</v>
+        <v>7.3548796</v>
       </c>
       <c r="R31" t="n">
-        <v>-1272.89342</v>
+        <v>-1470.97592</v>
       </c>
       <c r="S31" t="n">
-        <v>-55.98658</v>
+        <v>-102.02408</v>
       </c>
       <c r="T31" t="inlineStr">
         <is>
@@ -3045,7 +3045,7 @@
         </is>
       </c>
       <c r="V31" t="n">
-        <v>-1328.88</v>
+        <v>-1573</v>
       </c>
     </row>
     <row r="32">
@@ -3064,7 +3064,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>OPT</t>
+          <t>FOP</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -3074,23 +3074,23 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>SPY   261218P00505000</t>
+          <t>EW2G6 P6625</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>SPY 18DEC26 505 P</t>
+          <t>ES 13FEB26 6625 P</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I32" t="n">
-        <v>505</v>
+        <v>6625</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-12-18</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3100,29 +3100,29 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M32" t="n">
         <v>-2</v>
       </c>
       <c r="N32" t="n">
-        <v>7.645</v>
+        <v>13.5</v>
       </c>
       <c r="O32" t="n">
-        <v>-1529</v>
+        <v>-1350</v>
       </c>
       <c r="P32" t="n">
-        <v>7.3548796</v>
+        <v>42.2216</v>
       </c>
       <c r="Q32" t="n">
-        <v>7.3548796</v>
+        <v>42.2216</v>
       </c>
       <c r="R32" t="n">
-        <v>-1470.97592</v>
+        <v>-4222.16</v>
       </c>
       <c r="S32" t="n">
-        <v>-58.02408</v>
+        <v>2872.16</v>
       </c>
       <c r="T32" t="inlineStr">
         <is>
@@ -3131,11 +3131,11 @@
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>CBOE</t>
+          <t>CME</t>
         </is>
       </c>
       <c r="V32" t="n">
-        <v>-1529</v>
+        <v>-1350</v>
       </c>
     </row>
     <row r="33">
@@ -3159,24 +3159,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>EW2G6 P6625</t>
+          <t>EW2G6 C7200</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>ES 13FEB26 6625 P</t>
+          <t>ES 13FEB26 7200 C</t>
         </is>
       </c>
       <c r="H33" t="n">
         <v>50</v>
       </c>
       <c r="I33" t="n">
-        <v>6625</v>
+        <v>7200</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3185,34 +3185,34 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M33" t="n">
         <v>-2</v>
       </c>
       <c r="N33" t="n">
-        <v>12.5</v>
+        <v>2.15</v>
       </c>
       <c r="O33" t="n">
-        <v>-1250</v>
+        <v>-215</v>
       </c>
       <c r="P33" t="n">
-        <v>42.2216</v>
+        <v>18.9716</v>
       </c>
       <c r="Q33" t="n">
-        <v>42.2216</v>
+        <v>18.9716</v>
       </c>
       <c r="R33" t="n">
-        <v>-4222.16</v>
+        <v>-1897.16</v>
       </c>
       <c r="S33" t="n">
-        <v>2972.16</v>
+        <v>1682.16</v>
       </c>
       <c r="T33" t="inlineStr">
         <is>
@@ -3225,97 +3225,7 @@
         </is>
       </c>
       <c r="V33" t="n">
-        <v>-1250</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>U2739721</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>1</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>FOP</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>EW2G6 C7200</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>ES 13FEB26 7200 C</t>
-        </is>
-      </c>
-      <c r="H34" t="n">
-        <v>50</v>
-      </c>
-      <c r="I34" t="n">
-        <v>7200</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>2026-02-13</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>2026-01-29</t>
-        </is>
-      </c>
-      <c r="M34" t="n">
-        <v>-2</v>
-      </c>
-      <c r="N34" t="n">
-        <v>4.05</v>
-      </c>
-      <c r="O34" t="n">
-        <v>-405</v>
-      </c>
-      <c r="P34" t="n">
-        <v>18.9716</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>18.9716</v>
-      </c>
-      <c r="R34" t="n">
-        <v>-1897.16</v>
-      </c>
-      <c r="S34" t="n">
-        <v>1492.16</v>
-      </c>
-      <c r="T34" t="inlineStr">
-        <is>
-          <t>Short</t>
-        </is>
-      </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>CME</t>
-        </is>
-      </c>
-      <c r="V34" t="n">
-        <v>-405</v>
+        <v>-215</v>
       </c>
     </row>
   </sheetData>
@@ -3329,7 +3239,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3461,7 +3371,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.3084</v>
+        <v>1.2935</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -3491,17 +3401,17 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M2" t="n">
         <v>50</v>
       </c>
       <c r="N2" t="n">
-        <v>410.05</v>
+        <v>411.6</v>
       </c>
       <c r="O2" t="n">
-        <v>20502.5</v>
+        <v>20580</v>
       </c>
       <c r="P2" t="n">
         <v>419.6591247</v>
@@ -3513,7 +3423,7 @@
         <v>20982.956235</v>
       </c>
       <c r="S2" t="n">
-        <v>-480.456235</v>
+        <v>-402.956235</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
@@ -3526,7 +3436,7 @@
         </is>
       </c>
       <c r="V2" t="n">
-        <v>26825.471</v>
+        <v>26620.23</v>
       </c>
     </row>
     <row r="3">
@@ -3541,7 +3451,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.3084</v>
+        <v>1.2935</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -3571,17 +3481,17 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M3" t="n">
         <v>5500</v>
       </c>
       <c r="N3" t="n">
-        <v>3.5335</v>
+        <v>3.5425</v>
       </c>
       <c r="O3" t="n">
-        <v>19434.25</v>
+        <v>19483.75</v>
       </c>
       <c r="P3" t="n">
         <v>3.57708765</v>
@@ -3593,7 +3503,7 @@
         <v>19673.982075</v>
       </c>
       <c r="S3" t="n">
-        <v>-239.732075</v>
+        <v>-190.232075</v>
       </c>
       <c r="T3" t="inlineStr">
         <is>
@@ -3606,7 +3516,7 @@
         </is>
       </c>
       <c r="V3" t="n">
-        <v>25427.7727</v>
+        <v>25202.230625</v>
       </c>
     </row>
     <row r="4">
@@ -3621,7 +3531,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.3084</v>
+        <v>1.2935</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -3651,17 +3561,17 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M4" t="n">
         <v>200</v>
       </c>
       <c r="N4" t="n">
-        <v>63.64</v>
+        <v>63.41</v>
       </c>
       <c r="O4" t="n">
-        <v>12728</v>
+        <v>12682</v>
       </c>
       <c r="P4" t="n">
         <v>64.6234956</v>
@@ -3673,7 +3583,7 @@
         <v>12924.69912</v>
       </c>
       <c r="S4" t="n">
-        <v>-196.69912</v>
+        <v>-242.69912</v>
       </c>
       <c r="T4" t="inlineStr">
         <is>
@@ -3686,7 +3596,7 @@
         </is>
       </c>
       <c r="V4" t="n">
-        <v>16653.3152</v>
+        <v>16404.167</v>
       </c>
     </row>
     <row r="5">
@@ -3701,7 +3611,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.14399</v>
+        <v>0.1437</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -3731,17 +3641,17 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M5" t="n">
         <v>2000</v>
       </c>
       <c r="N5" t="n">
-        <v>31.92</v>
+        <v>31.58</v>
       </c>
       <c r="O5" t="n">
-        <v>63840</v>
+        <v>63160</v>
       </c>
       <c r="P5" t="n">
         <v>31.696238595</v>
@@ -3753,7 +3663,7 @@
         <v>63392.47719</v>
       </c>
       <c r="S5" t="n">
-        <v>447.52281</v>
+        <v>-232.47719</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -3766,7 +3676,7 @@
         </is>
       </c>
       <c r="V5" t="n">
-        <v>9192.321600000001</v>
+        <v>9076.092000000001</v>
       </c>
     </row>
     <row r="6">
@@ -3781,7 +3691,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.1971</v>
+        <v>1.185</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -3811,17 +3721,17 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M6" t="n">
         <v>4000</v>
       </c>
       <c r="N6" t="n">
-        <v>4.5805</v>
+        <v>4.5705</v>
       </c>
       <c r="O6" t="n">
-        <v>18322</v>
+        <v>18282</v>
       </c>
       <c r="P6" t="n">
         <v>4.65882825</v>
@@ -3833,7 +3743,7 @@
         <v>18635.313</v>
       </c>
       <c r="S6" t="n">
-        <v>-313.313</v>
+        <v>-353.313</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
@@ -3846,7 +3756,7 @@
         </is>
       </c>
       <c r="V6" t="n">
-        <v>21933.2662</v>
+        <v>21664.17</v>
       </c>
     </row>
     <row r="7">
@@ -3861,7 +3771,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.1971</v>
+        <v>1.185</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -3891,17 +3801,17 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M7" t="n">
         <v>1000</v>
       </c>
       <c r="N7" t="n">
-        <v>46.88</v>
+        <v>47.32</v>
       </c>
       <c r="O7" t="n">
-        <v>46880</v>
+        <v>47320</v>
       </c>
       <c r="P7" t="n">
         <v>43.01</v>
@@ -3913,7 +3823,7 @@
         <v>43010</v>
       </c>
       <c r="S7" t="n">
-        <v>3870</v>
+        <v>4310</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
@@ -3926,7 +3836,7 @@
         </is>
       </c>
       <c r="V7" t="n">
-        <v>56120.048</v>
+        <v>56074.2</v>
       </c>
     </row>
     <row r="8">
@@ -3941,7 +3851,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.79082</v>
+        <v>0.78593</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -3971,17 +3881,17 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M8" t="n">
         <v>10000</v>
       </c>
       <c r="N8" t="n">
-        <v>5.019</v>
+        <v>4.996</v>
       </c>
       <c r="O8" t="n">
-        <v>50190</v>
+        <v>49960</v>
       </c>
       <c r="P8" t="n">
         <v>3.81181816</v>
@@ -3993,7 +3903,7 @@
         <v>38118.1816</v>
       </c>
       <c r="S8" t="n">
-        <v>12071.8184</v>
+        <v>11841.8184</v>
       </c>
       <c r="T8" t="inlineStr">
         <is>
@@ -4006,7 +3916,7 @@
         </is>
       </c>
       <c r="V8" t="n">
-        <v>39691.2558</v>
+        <v>39265.0628</v>
       </c>
     </row>
     <row r="9">
@@ -4017,11 +3927,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.79082</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -4035,12 +3945,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>GSD</t>
+          <t>BITO</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>SPDR GOLD SHARES</t>
+          <t>PROSHARES BITCOIN ETF-USD</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -4051,29 +3961,29 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="N9" t="n">
-        <v>640.2</v>
+        <v>11.6</v>
       </c>
       <c r="O9" t="n">
-        <v>32010</v>
+        <v>2320</v>
       </c>
       <c r="P9" t="n">
-        <v>593.7864108799999</v>
+        <v>12.7</v>
       </c>
       <c r="Q9" t="n">
-        <v>593.7864108799999</v>
+        <v>12.7</v>
       </c>
       <c r="R9" t="n">
-        <v>29689.320544</v>
+        <v>2540</v>
       </c>
       <c r="S9" t="n">
-        <v>2320.679456</v>
+        <v>-220</v>
       </c>
       <c r="T9" t="inlineStr">
         <is>
@@ -4082,11 +3992,11 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>SGX</t>
+          <t>ARCA</t>
         </is>
       </c>
       <c r="V9" t="n">
-        <v>25314.1482</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="10">
@@ -4115,12 +4025,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>BITO</t>
+          <t>CSNDX</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>PROSHARES BITCOIN ETF-USD</t>
+          <t>ISHARES NASDAQ 100 USD ACC</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -4131,29 +4041,29 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="N10" t="n">
-        <v>11.66</v>
+        <v>1474.8</v>
       </c>
       <c r="O10" t="n">
-        <v>2332</v>
+        <v>29496</v>
       </c>
       <c r="P10" t="n">
-        <v>12.7</v>
+        <v>1467.02705</v>
       </c>
       <c r="Q10" t="n">
-        <v>12.7</v>
+        <v>1467.02705</v>
       </c>
       <c r="R10" t="n">
-        <v>2540</v>
+        <v>29340.541</v>
       </c>
       <c r="S10" t="n">
-        <v>-208</v>
+        <v>155.459</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -4162,11 +4072,11 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>ARCA</t>
+          <t>EBS</t>
         </is>
       </c>
       <c r="V10" t="n">
-        <v>2332</v>
+        <v>29496</v>
       </c>
     </row>
     <row r="11">
@@ -4190,17 +4100,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>CSNDX</t>
+          <t>GOOGL</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ISHARES NASDAQ 100 USD ACC</t>
+          <t>ALPHABET INC-CL A</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -4211,29 +4121,29 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="N11" t="n">
-        <v>1466.4</v>
+        <v>338</v>
       </c>
       <c r="O11" t="n">
-        <v>29328</v>
+        <v>33800</v>
       </c>
       <c r="P11" t="n">
-        <v>1467.02705</v>
+        <v>331.87755</v>
       </c>
       <c r="Q11" t="n">
-        <v>1467.02705</v>
+        <v>331.87755</v>
       </c>
       <c r="R11" t="n">
-        <v>29340.541</v>
+        <v>33187.755</v>
       </c>
       <c r="S11" t="n">
-        <v>-12.541</v>
+        <v>612.245</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -4242,11 +4152,11 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>EBS</t>
+          <t>NASDAQ</t>
         </is>
       </c>
       <c r="V11" t="n">
-        <v>29328</v>
+        <v>33800</v>
       </c>
     </row>
     <row r="12">
@@ -4270,17 +4180,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>GOOGL</t>
+          <t>HEAL</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>ALPHABET INC-CL A</t>
+          <t>ISHR HEALTHCARE INNOVATION</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -4291,29 +4201,29 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="N12" t="n">
-        <v>338.25</v>
+        <v>9.2925</v>
       </c>
       <c r="O12" t="n">
-        <v>33825</v>
+        <v>9292.5</v>
       </c>
       <c r="P12" t="n">
-        <v>331.87755</v>
+        <v>9.405900600000001</v>
       </c>
       <c r="Q12" t="n">
-        <v>331.87755</v>
+        <v>9.405900600000001</v>
       </c>
       <c r="R12" t="n">
-        <v>33187.755</v>
+        <v>9405.900600000001</v>
       </c>
       <c r="S12" t="n">
-        <v>637.245</v>
+        <v>-113.4006</v>
       </c>
       <c r="T12" t="inlineStr">
         <is>
@@ -4322,11 +4232,11 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>LSEETF</t>
         </is>
       </c>
       <c r="V12" t="n">
-        <v>33825</v>
+        <v>9292.5</v>
       </c>
     </row>
     <row r="13">
@@ -4350,17 +4260,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>HEAL</t>
+          <t>IBKR</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>ISHR HEALTHCARE INNOVATION</t>
+          <t>INTERACTIVE BROKERS GRO-CL A</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -4371,29 +4281,29 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>1000</v>
+        <v>16.8448</v>
       </c>
       <c r="N13" t="n">
-        <v>9.3725</v>
+        <v>74.88</v>
       </c>
       <c r="O13" t="n">
-        <v>9372.5</v>
+        <v>1261.34</v>
       </c>
       <c r="P13" t="n">
-        <v>9.405900600000001</v>
+        <v>20.721325216</v>
       </c>
       <c r="Q13" t="n">
-        <v>9.405900600000001</v>
+        <v>20.721325216</v>
       </c>
       <c r="R13" t="n">
-        <v>9405.900600000001</v>
+        <v>349.046579</v>
       </c>
       <c r="S13" t="n">
-        <v>-33.4006</v>
+        <v>912.293421</v>
       </c>
       <c r="T13" t="inlineStr">
         <is>
@@ -4402,11 +4312,11 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>LSEETF</t>
+          <t>NASDAQ</t>
         </is>
       </c>
       <c r="V13" t="n">
-        <v>9372.5</v>
+        <v>1261.34</v>
       </c>
     </row>
     <row r="14">
@@ -4430,17 +4340,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>IBKR</t>
+          <t>INRA</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>INTERACTIVE BROKERS GRO-CL A</t>
+          <t>ISHAR GL CL EN TR UCI ETF-US</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -4451,29 +4361,29 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>16.8448</v>
+        <v>385</v>
       </c>
       <c r="N14" t="n">
-        <v>75.66</v>
+        <v>27.0617</v>
       </c>
       <c r="O14" t="n">
-        <v>1274.48</v>
+        <v>10418.75</v>
       </c>
       <c r="P14" t="n">
-        <v>20.721325216</v>
+        <v>25.997158151</v>
       </c>
       <c r="Q14" t="n">
-        <v>20.721325216</v>
+        <v>25.997158151</v>
       </c>
       <c r="R14" t="n">
-        <v>349.046579</v>
+        <v>10008.905888</v>
       </c>
       <c r="S14" t="n">
-        <v>925.433421</v>
+        <v>409.844112</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
@@ -4482,11 +4392,11 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>NASDAQ</t>
+          <t>AEB</t>
         </is>
       </c>
       <c r="V14" t="n">
-        <v>1274.48</v>
+        <v>10418.75</v>
       </c>
     </row>
     <row r="15">
@@ -4510,17 +4420,17 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>COMMON</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>INRA</t>
+          <t>JPM</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ISHAR GL CL EN TR UCI ETF-US</t>
+          <t>JPMORGAN CHASE &amp; CO</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -4531,29 +4441,29 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>385</v>
+        <v>100</v>
       </c>
       <c r="N15" t="n">
-        <v>27.0739</v>
+        <v>305.89</v>
       </c>
       <c r="O15" t="n">
-        <v>10423.45</v>
+        <v>30589</v>
       </c>
       <c r="P15" t="n">
-        <v>25.997158151</v>
+        <v>298.02</v>
       </c>
       <c r="Q15" t="n">
-        <v>25.997158151</v>
+        <v>298.02</v>
       </c>
       <c r="R15" t="n">
-        <v>10008.905888</v>
+        <v>29802</v>
       </c>
       <c r="S15" t="n">
-        <v>414.544112</v>
+        <v>787</v>
       </c>
       <c r="T15" t="inlineStr">
         <is>
@@ -4562,11 +4472,11 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>AEB</t>
+          <t>NYSE</t>
         </is>
       </c>
       <c r="V15" t="n">
-        <v>10423.45</v>
+        <v>30589</v>
       </c>
     </row>
     <row r="16">
@@ -4590,17 +4500,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>COMMON</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>JPM</t>
+          <t>LOCK</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>JPMORGAN CHASE &amp; CO</t>
+          <t>ISHARES DIGITAL SCRTY USD-A</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -4611,29 +4521,29 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="N16" t="n">
-        <v>306.42</v>
+        <v>9.824</v>
       </c>
       <c r="O16" t="n">
-        <v>30642</v>
+        <v>9824</v>
       </c>
       <c r="P16" t="n">
-        <v>298.02</v>
+        <v>10.229112</v>
       </c>
       <c r="Q16" t="n">
-        <v>298.02</v>
+        <v>10.229112</v>
       </c>
       <c r="R16" t="n">
-        <v>29802</v>
+        <v>10229.112</v>
       </c>
       <c r="S16" t="n">
-        <v>840</v>
+        <v>-405.112</v>
       </c>
       <c r="T16" t="inlineStr">
         <is>
@@ -4642,11 +4552,11 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>NYSE</t>
+          <t>LSEETF</t>
         </is>
       </c>
       <c r="V16" t="n">
-        <v>30642</v>
+        <v>9824</v>
       </c>
     </row>
     <row r="17">
@@ -4675,12 +4585,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>LOCK</t>
+          <t>VWRA</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>ISHARES DIGITAL SCRTY USD-A</t>
+          <t>VANG FTSE AW USDA</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -4691,29 +4601,29 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="N17" t="n">
-        <v>9.85</v>
+        <v>174.7</v>
       </c>
       <c r="O17" t="n">
-        <v>9850</v>
+        <v>52410</v>
       </c>
       <c r="P17" t="n">
-        <v>10.229112</v>
+        <v>172.7421946</v>
       </c>
       <c r="Q17" t="n">
-        <v>10.229112</v>
+        <v>172.7421946</v>
       </c>
       <c r="R17" t="n">
-        <v>10229.112</v>
+        <v>51822.65838</v>
       </c>
       <c r="S17" t="n">
-        <v>-379.112</v>
+        <v>587.34162</v>
       </c>
       <c r="T17" t="inlineStr">
         <is>
@@ -4726,7 +4636,7 @@
         </is>
       </c>
       <c r="V17" t="n">
-        <v>9850</v>
+        <v>52410</v>
       </c>
     </row>
     <row r="18">
@@ -4745,55 +4655,65 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>OPT</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>VWRA</t>
+          <t>QQQ   261218P00560000</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>VANG FTSE AW USDA</t>
+          <t>QQQ 18DEC26 560 P</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
-      </c>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+        <v>100</v>
+      </c>
+      <c r="I18" t="n">
+        <v>560</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2026-12-18</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="N18" t="n">
-        <v>174.54</v>
+        <v>25.8147</v>
       </c>
       <c r="O18" t="n">
-        <v>52362</v>
+        <v>5162.94</v>
       </c>
       <c r="P18" t="n">
-        <v>172.7421946</v>
+        <v>23.5270125</v>
       </c>
       <c r="Q18" t="n">
-        <v>172.7421946</v>
+        <v>23.5270125</v>
       </c>
       <c r="R18" t="n">
-        <v>51822.65838</v>
+        <v>4705.4025</v>
       </c>
       <c r="S18" t="n">
-        <v>539.34162</v>
+        <v>457.5375</v>
       </c>
       <c r="T18" t="inlineStr">
         <is>
@@ -4802,11 +4722,11 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>LSEETF</t>
+          <t>CBOE</t>
         </is>
       </c>
       <c r="V18" t="n">
-        <v>52362</v>
+        <v>5162.94</v>
       </c>
     </row>
     <row r="19">
@@ -4835,19 +4755,19 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>QQQ   261218P00560000</t>
+          <t>SPY   261218P00620000</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>QQQ 18DEC26 560 P</t>
+          <t>SPY 18DEC26 620 P</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>100</v>
       </c>
       <c r="I19" t="n">
-        <v>560</v>
+        <v>620</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -4861,29 +4781,29 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M19" t="n">
         <v>2</v>
       </c>
       <c r="N19" t="n">
-        <v>24.0436</v>
+        <v>21.1757</v>
       </c>
       <c r="O19" t="n">
-        <v>4808.72</v>
+        <v>4235.14</v>
       </c>
       <c r="P19" t="n">
-        <v>23.5270125</v>
+        <v>20.1350875</v>
       </c>
       <c r="Q19" t="n">
-        <v>23.5270125</v>
+        <v>20.1350875</v>
       </c>
       <c r="R19" t="n">
-        <v>4705.4025</v>
+        <v>4027.0175</v>
       </c>
       <c r="S19" t="n">
-        <v>103.3175</v>
+        <v>208.1225</v>
       </c>
       <c r="T19" t="inlineStr">
         <is>
@@ -4896,7 +4816,7 @@
         </is>
       </c>
       <c r="V19" t="n">
-        <v>4808.72</v>
+        <v>4235.14</v>
       </c>
     </row>
     <row r="20">
@@ -4920,64 +4840,64 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>SPY   261218P00620000</t>
+          <t>GOOGL 260206C00335000</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>SPY 18DEC26 620 P</t>
+          <t>GOOGL 06FEB26 335 C</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>100</v>
       </c>
       <c r="I20" t="n">
-        <v>620</v>
+        <v>335</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2026-12-18</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="N20" t="n">
-        <v>20.615</v>
+        <v>12.1073</v>
       </c>
       <c r="O20" t="n">
-        <v>4123</v>
+        <v>-1210.73</v>
       </c>
       <c r="P20" t="n">
-        <v>20.1350875</v>
+        <v>10.0494796</v>
       </c>
       <c r="Q20" t="n">
-        <v>20.1350875</v>
+        <v>10.0494796</v>
       </c>
       <c r="R20" t="n">
-        <v>4027.0175</v>
+        <v>-1004.94796</v>
       </c>
       <c r="S20" t="n">
-        <v>95.9825</v>
+        <v>-205.78204</v>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>Long</t>
+          <t>Short</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
@@ -4986,7 +4906,7 @@
         </is>
       </c>
       <c r="V20" t="n">
-        <v>4123</v>
+        <v>-1210.73</v>
       </c>
     </row>
     <row r="21">
@@ -5010,60 +4930,60 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>GOOGL 260206C00335000</t>
+          <t>GOOGL 260220P00315000</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>GOOGL 06FEB26 335 C</t>
+          <t>GOOGL 20FEB26 315 P</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>100</v>
       </c>
       <c r="I21" t="n">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M21" t="n">
         <v>-1</v>
       </c>
       <c r="N21" t="n">
-        <v>12.7125</v>
+        <v>4.4882</v>
       </c>
       <c r="O21" t="n">
-        <v>-1271.25</v>
+        <v>-448.82</v>
       </c>
       <c r="P21" t="n">
-        <v>10.0494796</v>
+        <v>8.729479599999999</v>
       </c>
       <c r="Q21" t="n">
-        <v>10.0494796</v>
+        <v>8.729479599999999</v>
       </c>
       <c r="R21" t="n">
-        <v>-1004.94796</v>
+        <v>-872.94796</v>
       </c>
       <c r="S21" t="n">
-        <v>-266.30204</v>
+        <v>424.12796</v>
       </c>
       <c r="T21" t="inlineStr">
         <is>
@@ -5076,7 +4996,7 @@
         </is>
       </c>
       <c r="V21" t="n">
-        <v>-1271.25</v>
+        <v>-448.82</v>
       </c>
     </row>
     <row r="22">
@@ -5100,17 +5020,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>GOOGL 260220P00315000</t>
+          <t>JPM   260206C00315000</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>GOOGL 20FEB26 315 P</t>
+          <t>JPM 06FEB26 315 C</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -5121,39 +5041,39 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M22" t="n">
         <v>-1</v>
       </c>
       <c r="N22" t="n">
-        <v>4.8</v>
+        <v>0.78</v>
       </c>
       <c r="O22" t="n">
-        <v>-480</v>
+        <v>-78</v>
       </c>
       <c r="P22" t="n">
-        <v>8.729479599999999</v>
+        <v>2.0294546</v>
       </c>
       <c r="Q22" t="n">
-        <v>8.729479599999999</v>
+        <v>2.0294546</v>
       </c>
       <c r="R22" t="n">
-        <v>-872.94796</v>
+        <v>-202.94546</v>
       </c>
       <c r="S22" t="n">
-        <v>392.94796</v>
+        <v>124.94546</v>
       </c>
       <c r="T22" t="inlineStr">
         <is>
@@ -5166,7 +5086,7 @@
         </is>
       </c>
       <c r="V22" t="n">
-        <v>-480</v>
+        <v>-78</v>
       </c>
     </row>
     <row r="23">
@@ -5190,60 +5110,60 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>JPM   260206C00315000</t>
+          <t>QQQ   261218P00425000</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>JPM 06FEB26 315 C</t>
+          <t>QQQ 18DEC26 425 P</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>100</v>
       </c>
       <c r="I23" t="n">
-        <v>315</v>
+        <v>425</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-12-18</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>P</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N23" t="n">
-        <v>1.22</v>
+        <v>7.1668</v>
       </c>
       <c r="O23" t="n">
-        <v>-122</v>
+        <v>-1433.36</v>
       </c>
       <c r="P23" t="n">
-        <v>2.0294546</v>
+        <v>6.3929546</v>
       </c>
       <c r="Q23" t="n">
-        <v>2.0294546</v>
+        <v>6.3929546</v>
       </c>
       <c r="R23" t="n">
-        <v>-202.94546</v>
+        <v>-1278.59092</v>
       </c>
       <c r="S23" t="n">
-        <v>80.94546</v>
+        <v>-154.76908</v>
       </c>
       <c r="T23" t="inlineStr">
         <is>
@@ -5256,7 +5176,7 @@
         </is>
       </c>
       <c r="V23" t="n">
-        <v>-122</v>
+        <v>-1433.36</v>
       </c>
     </row>
     <row r="24">
@@ -5285,55 +5205,55 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>QQQ   260130P00608000</t>
+          <t>SPY   261218P00505000</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>QQQ 30JAN26 608 P</t>
+          <t>SPY 18DEC26 505 P</t>
         </is>
       </c>
       <c r="H24" t="n">
         <v>100</v>
       </c>
       <c r="I24" t="n">
-        <v>608</v>
+        <v>505</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
+          <t>2026-12-18</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
           <t>2026-01-30</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>2026-01-29</t>
-        </is>
-      </c>
       <c r="M24" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="N24" t="n">
-        <v>0.08500000000000001</v>
+        <v>7.865</v>
       </c>
       <c r="O24" t="n">
-        <v>-8.5</v>
+        <v>-1573</v>
       </c>
       <c r="P24" t="n">
-        <v>6.0594796</v>
+        <v>7.3496796</v>
       </c>
       <c r="Q24" t="n">
-        <v>6.0594796</v>
+        <v>7.3496796</v>
       </c>
       <c r="R24" t="n">
-        <v>-605.94796</v>
+        <v>-1469.93592</v>
       </c>
       <c r="S24" t="n">
-        <v>597.44796</v>
+        <v>-103.06408</v>
       </c>
       <c r="T24" t="inlineStr">
         <is>
@@ -5346,187 +5266,7 @@
         </is>
       </c>
       <c r="V24" t="n">
-        <v>-8.5</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>U6565621</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>OPT</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>QQQ   261218P00425000</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>QQQ 18DEC26 425 P</t>
-        </is>
-      </c>
-      <c r="H25" t="n">
-        <v>100</v>
-      </c>
-      <c r="I25" t="n">
-        <v>425</v>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>2026-12-18</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>2026-01-29</t>
-        </is>
-      </c>
-      <c r="M25" t="n">
-        <v>-2</v>
-      </c>
-      <c r="N25" t="n">
-        <v>6.6444</v>
-      </c>
-      <c r="O25" t="n">
-        <v>-1328.88</v>
-      </c>
-      <c r="P25" t="n">
-        <v>6.3929546</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>6.3929546</v>
-      </c>
-      <c r="R25" t="n">
-        <v>-1278.59092</v>
-      </c>
-      <c r="S25" t="n">
-        <v>-50.28908</v>
-      </c>
-      <c r="T25" t="inlineStr">
-        <is>
-          <t>Short</t>
-        </is>
-      </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>CBOE</t>
-        </is>
-      </c>
-      <c r="V25" t="n">
-        <v>-1328.88</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>U6565621</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>OPT</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>SPY   261218P00505000</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>SPY 18DEC26 505 P</t>
-        </is>
-      </c>
-      <c r="H26" t="n">
-        <v>100</v>
-      </c>
-      <c r="I26" t="n">
-        <v>505</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>2026-12-18</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>2026-01-29</t>
-        </is>
-      </c>
-      <c r="M26" t="n">
-        <v>-2</v>
-      </c>
-      <c r="N26" t="n">
-        <v>7.645</v>
-      </c>
-      <c r="O26" t="n">
-        <v>-1529</v>
-      </c>
-      <c r="P26" t="n">
-        <v>7.3496796</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>7.3496796</v>
-      </c>
-      <c r="R26" t="n">
-        <v>-1469.93592</v>
-      </c>
-      <c r="S26" t="n">
-        <v>-59.06408</v>
-      </c>
-      <c r="T26" t="inlineStr">
-        <is>
-          <t>Short</t>
-        </is>
-      </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>CBOE</t>
-        </is>
-      </c>
-      <c r="V26" t="n">
-        <v>-1529</v>
+        <v>-1573</v>
       </c>
     </row>
   </sheetData>
@@ -5578,17 +5318,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$318,293.90</t>
+          <t>$311,790.50</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$134,409.76</t>
+          <t>$138,115.20</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$452,703.65</t>
+          <t>$449,905.71</t>
         </is>
       </c>
     </row>
@@ -5600,17 +5340,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$404,759.12</t>
+          <t>$378,371.91</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$158,827.53</t>
+          <t>$181,807.52</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$563,586.65</t>
+          <t>$560,179.43</t>
         </is>
       </c>
     </row>
@@ -5628,17 +5368,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$723,053.02</t>
+          <t>$690,162.42</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>$293,237.28</t>
+          <t>$319,922.72</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$1,016,290.30</t>
+          <t>$1,010,085.13</t>
         </is>
       </c>
     </row>
@@ -5691,14 +5431,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-31 09:33:17</t>
+          <t>2026-01-31 15:55:40</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>

</xml_diff>